<commit_message>
Last test to go
</commit_message>
<xml_diff>
--- a/UnitTests/RaportGeneratorTestData.xlsx
+++ b/UnitTests/RaportGeneratorTestData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Użytkownik\source\repos\WindowsFormsApp1\UnitTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9697106-8465-4A0F-B7D2-248898A5E548}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1C2942-1FCF-45EE-AA95-3C9020C16F2F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{91592E27-BDF5-4EBE-B96A-BEC0E890A090}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{91592E27-BDF5-4EBE-B96A-BEC0E890A090}"/>
   </bookViews>
   <sheets>
     <sheet name="By cid and rid" sheetId="1" r:id="rId1"/>
     <sheet name="By name" sheetId="2" r:id="rId2"/>
+    <sheet name="By name for cid" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -187,7 +188,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -276,15 +277,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -520,11 +512,87 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -532,127 +600,299 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="14" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="14" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="10" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="12" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="11" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="12" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -661,227 +901,76 @@
     <xf numFmtId="2" fontId="0" fillId="10" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="12" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="11" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="12" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="15" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="15" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="15" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="15" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="15" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="10" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="15" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="15" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -890,25 +979,13 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="15" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="15" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="15" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="15" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1228,7 +1305,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1285,18 +1362,18 @@
       <c r="E2" s="48">
         <v>5.56</v>
       </c>
-      <c r="F2" s="84">
-        <f>E2*D2</f>
+      <c r="F2" s="82">
+        <f t="shared" ref="F2:F21" si="0">E2*D2</f>
         <v>5.56</v>
       </c>
-      <c r="G2" s="87">
+      <c r="G2" s="113">
         <f>SUM(F2:F4)</f>
         <v>48.94</v>
       </c>
-      <c r="H2" s="87">
-        <v>2</v>
-      </c>
-      <c r="I2" s="90">
+      <c r="H2" s="119">
+        <v>2</v>
+      </c>
+      <c r="I2" s="116">
         <f>G2/H2</f>
         <v>24.47</v>
       </c>
@@ -1318,12 +1395,12 @@
         <v>7.23</v>
       </c>
       <c r="F3" s="7">
-        <f>E3*D3</f>
+        <f t="shared" si="0"/>
         <v>14.46</v>
       </c>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="91"/>
+      <c r="G3" s="114"/>
+      <c r="H3" s="120"/>
+      <c r="I3" s="117"/>
     </row>
     <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="50">
@@ -1342,15 +1419,15 @@
         <v>7.23</v>
       </c>
       <c r="F4" s="8">
-        <f>E4*D4</f>
+        <f t="shared" si="0"/>
         <v>28.92</v>
       </c>
-      <c r="G4" s="89"/>
-      <c r="H4" s="89"/>
-      <c r="I4" s="92"/>
+      <c r="G4" s="115"/>
+      <c r="H4" s="121"/>
+      <c r="I4" s="118"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="77">
+      <c r="A5" s="75">
         <v>2</v>
       </c>
       <c r="B5" s="14">
@@ -1365,24 +1442,24 @@
       <c r="E5" s="14">
         <v>1.31</v>
       </c>
-      <c r="F5" s="85">
-        <f>E5*D5</f>
+      <c r="F5" s="83">
+        <f t="shared" si="0"/>
         <v>2.62</v>
       </c>
-      <c r="G5" s="87">
+      <c r="G5" s="113">
         <f>SUM(F5:F9)</f>
         <v>64.77</v>
       </c>
-      <c r="H5" s="87">
-        <v>2</v>
-      </c>
-      <c r="I5" s="93">
+      <c r="H5" s="119">
+        <v>2</v>
+      </c>
+      <c r="I5" s="110">
         <f>G5/H5</f>
         <v>32.384999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="77">
+      <c r="A6" s="75">
         <v>2</v>
       </c>
       <c r="B6" s="14">
@@ -1397,16 +1474,16 @@
       <c r="E6" s="14">
         <v>1.31</v>
       </c>
-      <c r="F6" s="85">
-        <f>E6*D6</f>
+      <c r="F6" s="83">
+        <f t="shared" si="0"/>
         <v>2.62</v>
       </c>
-      <c r="G6" s="88"/>
-      <c r="H6" s="88"/>
-      <c r="I6" s="94"/>
+      <c r="G6" s="114"/>
+      <c r="H6" s="120"/>
+      <c r="I6" s="111"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="77">
+      <c r="A7" s="75">
         <v>2</v>
       </c>
       <c r="B7" s="14">
@@ -1421,16 +1498,16 @@
       <c r="E7" s="14">
         <v>1.31</v>
       </c>
-      <c r="F7" s="85">
-        <f>E7*D7</f>
+      <c r="F7" s="83">
+        <f t="shared" si="0"/>
         <v>3.93</v>
       </c>
-      <c r="G7" s="88"/>
-      <c r="H7" s="88"/>
-      <c r="I7" s="94"/>
+      <c r="G7" s="114"/>
+      <c r="H7" s="120"/>
+      <c r="I7" s="111"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="78">
+      <c r="A8" s="76">
         <v>2</v>
       </c>
       <c r="B8" s="32">
@@ -1446,15 +1523,15 @@
         <v>5.56</v>
       </c>
       <c r="F8" s="7">
-        <f>E8*D8</f>
+        <f t="shared" si="0"/>
         <v>22.24</v>
       </c>
-      <c r="G8" s="88"/>
-      <c r="H8" s="88"/>
-      <c r="I8" s="94"/>
+      <c r="G8" s="114"/>
+      <c r="H8" s="120"/>
+      <c r="I8" s="111"/>
     </row>
     <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="79">
+      <c r="A9" s="77">
         <v>2</v>
       </c>
       <c r="B9" s="53">
@@ -1470,12 +1547,12 @@
         <v>5.56</v>
       </c>
       <c r="F9" s="5">
-        <f>E9*D9</f>
+        <f t="shared" si="0"/>
         <v>33.36</v>
       </c>
-      <c r="G9" s="89"/>
-      <c r="H9" s="89"/>
-      <c r="I9" s="95"/>
+      <c r="G9" s="115"/>
+      <c r="H9" s="121"/>
+      <c r="I9" s="112"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="55">
@@ -1493,18 +1570,18 @@
       <c r="E10" s="56">
         <v>1.31</v>
       </c>
-      <c r="F10" s="84">
-        <f>E10*D10</f>
+      <c r="F10" s="82">
+        <f t="shared" si="0"/>
         <v>3.93</v>
       </c>
-      <c r="G10" s="87">
+      <c r="G10" s="113">
         <f>SUM(F10:F13)</f>
         <v>142.94999999999999</v>
       </c>
-      <c r="H10" s="87">
-        <v>2</v>
-      </c>
-      <c r="I10" s="93">
+      <c r="H10" s="119">
+        <v>2</v>
+      </c>
+      <c r="I10" s="110">
         <f>G10/H10</f>
         <v>71.474999999999994</v>
       </c>
@@ -1525,13 +1602,13 @@
       <c r="E11" s="17">
         <v>5.56</v>
       </c>
-      <c r="F11" s="86">
-        <f>E11*D11</f>
+      <c r="F11" s="84">
+        <f t="shared" si="0"/>
         <v>27.799999999999997</v>
       </c>
-      <c r="G11" s="88"/>
-      <c r="H11" s="88"/>
-      <c r="I11" s="94"/>
+      <c r="G11" s="114"/>
+      <c r="H11" s="120"/>
+      <c r="I11" s="111"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="58">
@@ -1550,12 +1627,12 @@
         <v>5.56</v>
       </c>
       <c r="F12" s="7">
-        <f>E12*D12</f>
+        <f t="shared" si="0"/>
         <v>38.919999999999995</v>
       </c>
-      <c r="G12" s="88"/>
-      <c r="H12" s="88"/>
-      <c r="I12" s="94"/>
+      <c r="G12" s="114"/>
+      <c r="H12" s="120"/>
+      <c r="I12" s="111"/>
     </row>
     <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="59">
@@ -1574,15 +1651,15 @@
         <v>7.23</v>
       </c>
       <c r="F13" s="6">
-        <f>E13*D13</f>
+        <f t="shared" si="0"/>
         <v>72.300000000000011</v>
       </c>
-      <c r="G13" s="89"/>
-      <c r="H13" s="89"/>
-      <c r="I13" s="95"/>
+      <c r="G13" s="115"/>
+      <c r="H13" s="121"/>
+      <c r="I13" s="112"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="80">
+      <c r="A14" s="78">
         <v>4</v>
       </c>
       <c r="B14" s="18">
@@ -1597,24 +1674,24 @@
       <c r="E14" s="18">
         <v>1.31</v>
       </c>
-      <c r="F14" s="85">
-        <f>E14*D14</f>
+      <c r="F14" s="83">
+        <f t="shared" si="0"/>
         <v>1.31</v>
       </c>
-      <c r="G14" s="87">
+      <c r="G14" s="113">
         <f>SUM(F14:F17)</f>
         <v>20.97</v>
       </c>
-      <c r="H14" s="87">
-        <v>2</v>
-      </c>
-      <c r="I14" s="93">
+      <c r="H14" s="119">
+        <v>2</v>
+      </c>
+      <c r="I14" s="110">
         <f>G14/H14</f>
         <v>10.484999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="81">
+      <c r="A15" s="79">
         <v>4</v>
       </c>
       <c r="B15" s="41">
@@ -1630,15 +1707,15 @@
         <v>5.56</v>
       </c>
       <c r="F15" s="7">
-        <f>E15*D15</f>
+        <f t="shared" si="0"/>
         <v>11.12</v>
       </c>
-      <c r="G15" s="88"/>
-      <c r="H15" s="88"/>
-      <c r="I15" s="94"/>
+      <c r="G15" s="114"/>
+      <c r="H15" s="120"/>
+      <c r="I15" s="111"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="82">
+      <c r="A16" s="80">
         <v>4</v>
       </c>
       <c r="B16" s="43">
@@ -1654,15 +1731,15 @@
         <v>1.31</v>
       </c>
       <c r="F16" s="5">
-        <f>E16*D16</f>
+        <f t="shared" si="0"/>
         <v>1.31</v>
       </c>
-      <c r="G16" s="88"/>
-      <c r="H16" s="88"/>
-      <c r="I16" s="94"/>
+      <c r="G16" s="114"/>
+      <c r="H16" s="120"/>
+      <c r="I16" s="111"/>
     </row>
     <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="83">
+      <c r="A17" s="81">
         <v>4</v>
       </c>
       <c r="B17" s="20">
@@ -1677,13 +1754,13 @@
       <c r="E17" s="21">
         <v>7.23</v>
       </c>
-      <c r="F17" s="85">
-        <f>E17*D17</f>
+      <c r="F17" s="83">
+        <f t="shared" si="0"/>
         <v>7.23</v>
       </c>
-      <c r="G17" s="89"/>
-      <c r="H17" s="89"/>
-      <c r="I17" s="95"/>
+      <c r="G17" s="115"/>
+      <c r="H17" s="121"/>
+      <c r="I17" s="112"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="65">
@@ -1701,18 +1778,18 @@
       <c r="E18" s="66">
         <v>1.31</v>
       </c>
-      <c r="F18" s="84">
-        <f>E18*D18</f>
+      <c r="F18" s="82">
+        <f t="shared" si="0"/>
         <v>1.31</v>
       </c>
-      <c r="G18" s="87">
+      <c r="G18" s="113">
         <f>SUM(F18:F20)</f>
         <v>20.83</v>
       </c>
-      <c r="H18" s="87">
-        <v>2</v>
-      </c>
-      <c r="I18" s="93">
+      <c r="H18" s="119">
+        <v>2</v>
+      </c>
+      <c r="I18" s="110">
         <f>G18/H18</f>
         <v>10.414999999999999</v>
       </c>
@@ -1734,12 +1811,12 @@
         <v>5.56</v>
       </c>
       <c r="F19" s="7">
-        <f>E19*D19</f>
+        <f t="shared" si="0"/>
         <v>11.12</v>
       </c>
-      <c r="G19" s="88"/>
-      <c r="H19" s="88"/>
-      <c r="I19" s="94"/>
+      <c r="G19" s="114"/>
+      <c r="H19" s="120"/>
+      <c r="I19" s="111"/>
     </row>
     <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="68">
@@ -1758,12 +1835,12 @@
         <v>4.2</v>
       </c>
       <c r="F20" s="6">
-        <f>E20*D20</f>
+        <f t="shared" si="0"/>
         <v>8.4</v>
       </c>
-      <c r="G20" s="89"/>
-      <c r="H20" s="89"/>
-      <c r="I20" s="95"/>
+      <c r="G20" s="115"/>
+      <c r="H20" s="121"/>
+      <c r="I20" s="112"/>
     </row>
     <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="71">
@@ -1782,18 +1859,18 @@
         <v>4.2</v>
       </c>
       <c r="F21" s="9">
-        <f>E21*D21</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="G21" s="74">
+      <c r="G21" s="108">
         <f>SUM(F21)</f>
         <v>21</v>
       </c>
-      <c r="H21" s="75">
-        <v>1</v>
-      </c>
-      <c r="I21" s="76">
-        <f t="shared" ref="I5:I22" si="0">G21/H21</f>
+      <c r="H21" s="109">
+        <v>1</v>
+      </c>
+      <c r="I21" s="74">
+        <f t="shared" ref="I21:I22" si="1">G21/H21</f>
         <v>21</v>
       </c>
     </row>
@@ -1810,7 +1887,7 @@
         <v>11</v>
       </c>
       <c r="I22" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>29.041818181818179</v>
       </c>
     </row>
@@ -1844,10 +1921,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D190C58-97B3-4FCC-8D31-8F1AF72C877A}">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1872,7 +1949,7 @@
       <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="96" t="s">
+      <c r="F1" s="85" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1892,12 +1969,12 @@
       <c r="E2" s="23">
         <v>1.31</v>
       </c>
-      <c r="F2" s="109">
+      <c r="F2" s="122">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="97">
+      <c r="A3" s="86">
         <v>2</v>
       </c>
       <c r="B3" s="13">
@@ -1912,7 +1989,7 @@
       <c r="E3" s="13">
         <v>1.31</v>
       </c>
-      <c r="F3" s="110"/>
+      <c r="F3" s="123"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="25">
@@ -1930,97 +2007,97 @@
       <c r="E4" s="26">
         <v>1.31</v>
       </c>
-      <c r="F4" s="110"/>
+      <c r="F4" s="123"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="98">
+      <c r="A5" s="87">
         <v>3</v>
       </c>
-      <c r="B5" s="99">
-        <v>1</v>
-      </c>
-      <c r="C5" s="99" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="99">
+      <c r="B5" s="88">
+        <v>1</v>
+      </c>
+      <c r="C5" s="88" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="88">
         <v>3</v>
       </c>
-      <c r="E5" s="99">
+      <c r="E5" s="88">
         <v>1.31</v>
       </c>
-      <c r="F5" s="110"/>
+      <c r="F5" s="123"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="98">
+      <c r="A6" s="87">
         <v>4</v>
       </c>
-      <c r="B6" s="99">
-        <v>1</v>
-      </c>
-      <c r="C6" s="99" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="99">
-        <v>1</v>
-      </c>
-      <c r="E6" s="99">
+      <c r="B6" s="88">
+        <v>1</v>
+      </c>
+      <c r="C6" s="88" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="88">
+        <v>1</v>
+      </c>
+      <c r="E6" s="88">
         <v>1.31</v>
       </c>
-      <c r="F6" s="110"/>
+      <c r="F6" s="123"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="98">
+      <c r="A7" s="87">
         <v>4</v>
       </c>
-      <c r="B7" s="99">
-        <v>2</v>
-      </c>
-      <c r="C7" s="99" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="99">
-        <v>1</v>
-      </c>
-      <c r="E7" s="99">
+      <c r="B7" s="88">
+        <v>2</v>
+      </c>
+      <c r="C7" s="88" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="88">
+        <v>1</v>
+      </c>
+      <c r="E7" s="88">
         <v>1.31</v>
       </c>
-      <c r="F7" s="110"/>
+      <c r="F7" s="123"/>
     </row>
     <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="98">
+      <c r="A8" s="87">
         <v>5</v>
       </c>
-      <c r="B8" s="99">
-        <v>1</v>
-      </c>
-      <c r="C8" s="99" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="99">
-        <v>1</v>
-      </c>
-      <c r="E8" s="99">
+      <c r="B8" s="88">
+        <v>1</v>
+      </c>
+      <c r="C8" s="88" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="88">
+        <v>1</v>
+      </c>
+      <c r="E8" s="88">
         <v>1.31</v>
       </c>
-      <c r="F8" s="111"/>
+      <c r="F8" s="124"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>1</v>
       </c>
-      <c r="B9" s="100">
-        <v>1</v>
-      </c>
-      <c r="C9" s="100" t="s">
+      <c r="B9" s="89">
+        <v>1</v>
+      </c>
+      <c r="C9" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="100">
-        <v>1</v>
-      </c>
-      <c r="E9" s="105">
+      <c r="D9" s="89">
+        <v>1</v>
+      </c>
+      <c r="E9" s="94">
         <v>5.56</v>
       </c>
-      <c r="F9" s="112">
+      <c r="F9" s="125">
         <v>6</v>
       </c>
     </row>
@@ -2028,37 +2105,37 @@
       <c r="A10" s="3">
         <v>2</v>
       </c>
-      <c r="B10" s="100">
-        <v>1</v>
-      </c>
-      <c r="C10" s="100" t="s">
+      <c r="B10" s="89">
+        <v>1</v>
+      </c>
+      <c r="C10" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="100">
+      <c r="D10" s="89">
         <v>4</v>
       </c>
-      <c r="E10" s="105">
+      <c r="E10" s="94">
         <v>5.56</v>
       </c>
-      <c r="F10" s="112"/>
+      <c r="F10" s="125"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>2</v>
       </c>
-      <c r="B11" s="100">
+      <c r="B11" s="89">
         <v>3</v>
       </c>
-      <c r="C11" s="100" t="s">
+      <c r="C11" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="D11" s="100">
+      <c r="D11" s="89">
         <v>6</v>
       </c>
-      <c r="E11" s="105">
+      <c r="E11" s="94">
         <v>5.56</v>
       </c>
-      <c r="F11" s="112"/>
+      <c r="F11" s="125"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="28">
@@ -2073,10 +2150,10 @@
       <c r="D12" s="29">
         <v>5</v>
       </c>
-      <c r="E12" s="106">
+      <c r="E12" s="95">
         <v>5.56</v>
       </c>
-      <c r="F12" s="112"/>
+      <c r="F12" s="125"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="31">
@@ -2094,135 +2171,135 @@
       <c r="E13" s="33">
         <v>5.56</v>
       </c>
-      <c r="F13" s="112"/>
+      <c r="F13" s="125"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>4</v>
       </c>
-      <c r="B14" s="100">
-        <v>1</v>
-      </c>
-      <c r="C14" s="100" t="s">
+      <c r="B14" s="89">
+        <v>1</v>
+      </c>
+      <c r="C14" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="100">
-        <v>2</v>
-      </c>
-      <c r="E14" s="105">
+      <c r="D14" s="89">
+        <v>2</v>
+      </c>
+      <c r="E14" s="94">
         <v>5.56</v>
       </c>
-      <c r="F14" s="112"/>
+      <c r="F14" s="125"/>
     </row>
     <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>5</v>
       </c>
-      <c r="B15" s="100">
-        <v>1</v>
-      </c>
-      <c r="C15" s="100" t="s">
+      <c r="B15" s="89">
+        <v>1</v>
+      </c>
+      <c r="C15" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="100">
-        <v>2</v>
-      </c>
-      <c r="E15" s="105">
+      <c r="D15" s="89">
+        <v>2</v>
+      </c>
+      <c r="E15" s="94">
         <v>5.56</v>
       </c>
-      <c r="F15" s="112"/>
+      <c r="F15" s="125"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="101">
-        <v>1</v>
-      </c>
-      <c r="B16" s="102">
-        <v>1</v>
-      </c>
-      <c r="C16" s="102" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="102">
-        <v>2</v>
-      </c>
-      <c r="E16" s="107">
+      <c r="A16" s="90">
+        <v>1</v>
+      </c>
+      <c r="B16" s="91">
+        <v>1</v>
+      </c>
+      <c r="C16" s="91" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="91">
+        <v>2</v>
+      </c>
+      <c r="E16" s="96">
         <v>7.23</v>
       </c>
-      <c r="F16" s="113">
+      <c r="F16" s="126">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="101">
-        <v>1</v>
-      </c>
-      <c r="B17" s="102">
+      <c r="A17" s="90">
+        <v>1</v>
+      </c>
+      <c r="B17" s="91">
         <v>7</v>
       </c>
-      <c r="C17" s="102" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" s="102">
+      <c r="C17" s="91" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="91">
         <v>4</v>
       </c>
-      <c r="E17" s="107">
+      <c r="E17" s="96">
         <v>7.23</v>
       </c>
-      <c r="F17" s="112"/>
+      <c r="F17" s="125"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="101">
+      <c r="A18" s="90">
         <v>3</v>
       </c>
-      <c r="B18" s="102">
-        <v>2</v>
-      </c>
-      <c r="C18" s="102" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" s="102">
+      <c r="B18" s="91">
+        <v>2</v>
+      </c>
+      <c r="C18" s="91" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="91">
         <v>10</v>
       </c>
-      <c r="E18" s="107">
+      <c r="E18" s="96">
         <v>7.23</v>
       </c>
-      <c r="F18" s="112"/>
+      <c r="F18" s="125"/>
     </row>
     <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="101">
+      <c r="A19" s="90">
         <v>4</v>
       </c>
-      <c r="B19" s="102">
-        <v>2</v>
-      </c>
-      <c r="C19" s="102" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" s="102">
-        <v>1</v>
-      </c>
-      <c r="E19" s="107">
+      <c r="B19" s="91">
+        <v>2</v>
+      </c>
+      <c r="C19" s="91" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="91">
+        <v>1</v>
+      </c>
+      <c r="E19" s="96">
         <v>7.23</v>
       </c>
-      <c r="F19" s="114"/>
+      <c r="F19" s="127"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="103">
+      <c r="A20" s="92">
         <v>5</v>
       </c>
-      <c r="B20" s="104">
-        <v>2</v>
-      </c>
-      <c r="C20" s="104" t="s">
+      <c r="B20" s="93">
+        <v>2</v>
+      </c>
+      <c r="C20" s="93" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="104">
-        <v>2</v>
-      </c>
-      <c r="E20" s="108">
+      <c r="D20" s="93">
+        <v>2</v>
+      </c>
+      <c r="E20" s="97">
         <v>4.2</v>
       </c>
-      <c r="F20" s="112">
+      <c r="F20" s="125">
         <v>2</v>
       </c>
     </row>
@@ -2242,418 +2319,10 @@
       <c r="E21" s="42">
         <v>4.2</v>
       </c>
-      <c r="F21" s="114"/>
+      <c r="F21" s="127"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F22" s="115"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F24" s="96" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="98">
-        <v>1</v>
-      </c>
-      <c r="B25" s="99">
-        <v>1</v>
-      </c>
-      <c r="C25" s="99" t="s">
-        <v>0</v>
-      </c>
-      <c r="D25" s="99">
-        <v>1</v>
-      </c>
-      <c r="E25" s="116">
-        <v>5.56</v>
-      </c>
-      <c r="F25" s="124">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="22">
-        <v>1</v>
-      </c>
-      <c r="B26" s="23">
-        <v>1</v>
-      </c>
-      <c r="C26" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="D26" s="23">
-        <v>2</v>
-      </c>
-      <c r="E26" s="24">
-        <v>7.23</v>
-      </c>
-      <c r="F26" s="121">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="25">
-        <v>1</v>
-      </c>
-      <c r="B27" s="26">
-        <v>7</v>
-      </c>
-      <c r="C27" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="D27" s="26">
-        <v>4</v>
-      </c>
-      <c r="E27" s="27">
-        <v>7.23</v>
-      </c>
-      <c r="F27" s="122"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="28">
-        <v>2</v>
-      </c>
-      <c r="B28" s="29">
-        <v>1</v>
-      </c>
-      <c r="C28" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="D28" s="29">
-        <v>2</v>
-      </c>
-      <c r="E28" s="29">
-        <v>1.31</v>
-      </c>
-      <c r="F28" s="121">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="30">
-        <v>2</v>
-      </c>
-      <c r="B29" s="14">
-        <v>1</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D29" s="14">
-        <v>2</v>
-      </c>
-      <c r="E29" s="14">
-        <v>1.31</v>
-      </c>
-      <c r="F29" s="123"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="31">
-        <v>2</v>
-      </c>
-      <c r="B30" s="32">
-        <v>1</v>
-      </c>
-      <c r="C30" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="D30" s="32">
-        <v>3</v>
-      </c>
-      <c r="E30" s="32">
-        <v>1.31</v>
-      </c>
-      <c r="F30" s="122"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="77">
-        <v>2</v>
-      </c>
-      <c r="B31" s="14">
-        <v>1</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="D31" s="14">
-        <v>4</v>
-      </c>
-      <c r="E31" s="15">
-        <v>5.56</v>
-      </c>
-      <c r="F31" s="126">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="77">
-        <v>2</v>
-      </c>
-      <c r="B32" s="14">
-        <v>3</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="D32" s="14">
-        <v>6</v>
-      </c>
-      <c r="E32" s="15">
-        <v>5.56</v>
-      </c>
-      <c r="F32" s="127"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="101">
-        <v>3</v>
-      </c>
-      <c r="B33" s="102">
-        <v>1</v>
-      </c>
-      <c r="C33" s="102" t="s">
-        <v>1</v>
-      </c>
-      <c r="D33" s="102">
-        <v>3</v>
-      </c>
-      <c r="E33" s="102">
-        <v>1.31</v>
-      </c>
-      <c r="F33" s="128">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="34">
-        <v>3</v>
-      </c>
-      <c r="B34" s="35">
-        <v>1</v>
-      </c>
-      <c r="C34" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="D34" s="35">
-        <v>5</v>
-      </c>
-      <c r="E34" s="117">
-        <v>5.56</v>
-      </c>
-      <c r="F34" s="126">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="36">
-        <v>3</v>
-      </c>
-      <c r="B35" s="37">
-        <v>1</v>
-      </c>
-      <c r="C35" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="D35" s="37">
-        <v>7</v>
-      </c>
-      <c r="E35" s="38">
-        <v>5.56</v>
-      </c>
-      <c r="F35" s="127"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="57">
-        <v>3</v>
-      </c>
-      <c r="B36" s="16">
-        <v>2</v>
-      </c>
-      <c r="C36" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="D36" s="16">
-        <v>10</v>
-      </c>
-      <c r="E36" s="17">
-        <v>7.23</v>
-      </c>
-      <c r="F36" s="125">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="39">
-        <v>4</v>
-      </c>
-      <c r="B37" s="40">
-        <v>1</v>
-      </c>
-      <c r="C37" s="40" t="s">
-        <v>1</v>
-      </c>
-      <c r="D37" s="40">
-        <v>1</v>
-      </c>
-      <c r="E37" s="40">
-        <v>1.31</v>
-      </c>
-      <c r="F37" s="126">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="4">
-        <v>4</v>
-      </c>
-      <c r="B38" s="41">
-        <v>2</v>
-      </c>
-      <c r="C38" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="D38" s="41">
-        <v>1</v>
-      </c>
-      <c r="E38" s="41">
-        <v>1.31</v>
-      </c>
-      <c r="F38" s="127"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="103">
-        <v>4</v>
-      </c>
-      <c r="B39" s="104">
-        <v>1</v>
-      </c>
-      <c r="C39" s="104" t="s">
-        <v>0</v>
-      </c>
-      <c r="D39" s="104">
-        <v>2</v>
-      </c>
-      <c r="E39" s="108">
-        <v>5.56</v>
-      </c>
-      <c r="F39" s="128">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="80">
-        <v>4</v>
-      </c>
-      <c r="B40" s="18">
-        <v>2</v>
-      </c>
-      <c r="C40" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D40" s="18">
-        <v>1</v>
-      </c>
-      <c r="E40" s="19">
-        <v>7.23</v>
-      </c>
-      <c r="F40" s="125">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="118">
-        <v>5</v>
-      </c>
-      <c r="B41" s="119">
-        <v>1</v>
-      </c>
-      <c r="C41" s="119" t="s">
-        <v>1</v>
-      </c>
-      <c r="D41" s="119">
-        <v>1</v>
-      </c>
-      <c r="E41" s="119">
-        <v>1.31</v>
-      </c>
-      <c r="F41" s="128">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="118">
-        <v>5</v>
-      </c>
-      <c r="B42" s="119">
-        <v>1</v>
-      </c>
-      <c r="C42" s="119" t="s">
-        <v>0</v>
-      </c>
-      <c r="D42" s="119">
-        <v>2</v>
-      </c>
-      <c r="E42" s="120">
-        <v>5.56</v>
-      </c>
-      <c r="F42" s="128">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="118">
-        <v>5</v>
-      </c>
-      <c r="B43" s="119">
-        <v>2</v>
-      </c>
-      <c r="C43" s="119" t="s">
-        <v>3</v>
-      </c>
-      <c r="D43" s="119">
-        <v>2</v>
-      </c>
-      <c r="E43" s="120">
-        <v>4.2</v>
-      </c>
-      <c r="F43" s="128">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="62">
-        <v>6</v>
-      </c>
-      <c r="B44" s="63">
-        <v>6</v>
-      </c>
-      <c r="C44" s="63" t="s">
-        <v>3</v>
-      </c>
-      <c r="D44" s="63">
-        <v>5</v>
-      </c>
-      <c r="E44" s="64">
-        <v>4.2</v>
-      </c>
-      <c r="F44" s="129">
-        <v>1</v>
-      </c>
+      <c r="F22" s="98"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A25:E44">
@@ -2662,12 +2331,7 @@
     <sortCondition ref="B25:B44"/>
     <sortCondition ref="D25:D44"/>
   </sortState>
-  <mergeCells count="9">
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="F28:F30"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="F37:F38"/>
+  <mergeCells count="4">
     <mergeCell ref="F2:F8"/>
     <mergeCell ref="F9:F15"/>
     <mergeCell ref="F16:F19"/>
@@ -2675,4 +2339,439 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{278C7FD2-399F-4D80-8AD7-B7131F055316}">
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="85" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="87">
+        <v>1</v>
+      </c>
+      <c r="B2" s="88">
+        <v>1</v>
+      </c>
+      <c r="C2" s="88" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="88">
+        <v>1</v>
+      </c>
+      <c r="E2" s="99">
+        <v>5.56</v>
+      </c>
+      <c r="F2" s="104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="22">
+        <v>1</v>
+      </c>
+      <c r="B3" s="23">
+        <v>1</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="23">
+        <v>2</v>
+      </c>
+      <c r="E3" s="24">
+        <v>7.23</v>
+      </c>
+      <c r="F3" s="128">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="25">
+        <v>1</v>
+      </c>
+      <c r="B4" s="26">
+        <v>7</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="26">
+        <v>4</v>
+      </c>
+      <c r="E4" s="27">
+        <v>7.23</v>
+      </c>
+      <c r="F4" s="129"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="28">
+        <v>2</v>
+      </c>
+      <c r="B5" s="29">
+        <v>1</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="29">
+        <v>2</v>
+      </c>
+      <c r="E5" s="29">
+        <v>1.31</v>
+      </c>
+      <c r="F5" s="128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="30">
+        <v>2</v>
+      </c>
+      <c r="B6" s="14">
+        <v>1</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="14">
+        <v>2</v>
+      </c>
+      <c r="E6" s="14">
+        <v>1.31</v>
+      </c>
+      <c r="F6" s="130"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="31">
+        <v>2</v>
+      </c>
+      <c r="B7" s="32">
+        <v>1</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="32">
+        <v>3</v>
+      </c>
+      <c r="E7" s="32">
+        <v>1.31</v>
+      </c>
+      <c r="F7" s="129"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="75">
+        <v>2</v>
+      </c>
+      <c r="B8" s="14">
+        <v>1</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="14">
+        <v>4</v>
+      </c>
+      <c r="E8" s="15">
+        <v>5.56</v>
+      </c>
+      <c r="F8" s="131">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="75">
+        <v>2</v>
+      </c>
+      <c r="B9" s="14">
+        <v>3</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="14">
+        <v>6</v>
+      </c>
+      <c r="E9" s="15">
+        <v>5.56</v>
+      </c>
+      <c r="F9" s="132"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="90">
+        <v>3</v>
+      </c>
+      <c r="B10" s="91">
+        <v>1</v>
+      </c>
+      <c r="C10" s="91" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="91">
+        <v>3</v>
+      </c>
+      <c r="E10" s="91">
+        <v>1.31</v>
+      </c>
+      <c r="F10" s="107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="34">
+        <v>3</v>
+      </c>
+      <c r="B11" s="35">
+        <v>1</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="35">
+        <v>5</v>
+      </c>
+      <c r="E11" s="100">
+        <v>5.56</v>
+      </c>
+      <c r="F11" s="131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="36">
+        <v>3</v>
+      </c>
+      <c r="B12" s="37">
+        <v>1</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="37">
+        <v>7</v>
+      </c>
+      <c r="E12" s="38">
+        <v>5.56</v>
+      </c>
+      <c r="F12" s="132"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="57">
+        <v>3</v>
+      </c>
+      <c r="B13" s="16">
+        <v>2</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="16">
+        <v>10</v>
+      </c>
+      <c r="E13" s="17">
+        <v>7.23</v>
+      </c>
+      <c r="F13" s="105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="39">
+        <v>4</v>
+      </c>
+      <c r="B14" s="40">
+        <v>1</v>
+      </c>
+      <c r="C14" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="40">
+        <v>1</v>
+      </c>
+      <c r="E14" s="40">
+        <v>1.31</v>
+      </c>
+      <c r="F14" s="131">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
+        <v>4</v>
+      </c>
+      <c r="B15" s="41">
+        <v>2</v>
+      </c>
+      <c r="C15" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="41">
+        <v>1</v>
+      </c>
+      <c r="E15" s="41">
+        <v>1.31</v>
+      </c>
+      <c r="F15" s="132"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="92">
+        <v>4</v>
+      </c>
+      <c r="B16" s="93">
+        <v>1</v>
+      </c>
+      <c r="C16" s="93" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="93">
+        <v>2</v>
+      </c>
+      <c r="E16" s="97">
+        <v>5.56</v>
+      </c>
+      <c r="F16" s="107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="78">
+        <v>4</v>
+      </c>
+      <c r="B17" s="18">
+        <v>2</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="18">
+        <v>1</v>
+      </c>
+      <c r="E17" s="19">
+        <v>7.23</v>
+      </c>
+      <c r="F17" s="105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="101">
+        <v>5</v>
+      </c>
+      <c r="B18" s="102">
+        <v>1</v>
+      </c>
+      <c r="C18" s="102" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="102">
+        <v>1</v>
+      </c>
+      <c r="E18" s="102">
+        <v>1.31</v>
+      </c>
+      <c r="F18" s="107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="101">
+        <v>5</v>
+      </c>
+      <c r="B19" s="102">
+        <v>1</v>
+      </c>
+      <c r="C19" s="102" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="102">
+        <v>2</v>
+      </c>
+      <c r="E19" s="103">
+        <v>5.56</v>
+      </c>
+      <c r="F19" s="107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="101">
+        <v>5</v>
+      </c>
+      <c r="B20" s="102">
+        <v>2</v>
+      </c>
+      <c r="C20" s="102" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="102">
+        <v>2</v>
+      </c>
+      <c r="E20" s="103">
+        <v>4.2</v>
+      </c>
+      <c r="F20" s="107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="62">
+        <v>6</v>
+      </c>
+      <c r="B21" s="63">
+        <v>6</v>
+      </c>
+      <c r="C21" s="63" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="63">
+        <v>5</v>
+      </c>
+      <c r="E21" s="64">
+        <v>4.2</v>
+      </c>
+      <c r="F21" s="106">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F14:F15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
All RaportGenerator tests work and are passed, minor bug fixes in main app
</commit_message>
<xml_diff>
--- a/UnitTests/RaportGeneratorTestData.xlsx
+++ b/UnitTests/RaportGeneratorTestData.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Użytkownik\source\repos\WindowsFormsApp1\UnitTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1C2942-1FCF-45EE-AA95-3C9020C16F2F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60BAEC4-7944-4BCB-877B-4B40A2FB567A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{91592E27-BDF5-4EBE-B96A-BEC0E890A090}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{91592E27-BDF5-4EBE-B96A-BEC0E890A090}"/>
   </bookViews>
   <sheets>
     <sheet name="By cid and rid" sheetId="1" r:id="rId1"/>
-    <sheet name="By name" sheetId="2" r:id="rId2"/>
-    <sheet name="By name for cid" sheetId="3" r:id="rId3"/>
+    <sheet name="By ReqSum" sheetId="4" r:id="rId2"/>
+    <sheet name="By name" sheetId="2" r:id="rId3"/>
+    <sheet name="By name for cid" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="14">
   <si>
     <t>Chleb</t>
   </si>
@@ -72,6 +73,9 @@
   </si>
   <si>
     <t>Avg</t>
+  </si>
+  <si>
+    <t>ReqSum</t>
   </si>
 </sst>
 </file>
@@ -188,7 +192,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="50">
     <border>
       <left/>
       <right/>
@@ -256,37 +260,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -588,11 +561,261 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="200">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -600,34 +823,34 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="14" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="14" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -657,254 +880,254 @@
     <xf numFmtId="2" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="10" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="10" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="7" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="12" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="12" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="11" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="12" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="11" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="12" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="10" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="10" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="15" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="15" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="15" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -913,79 +1136,280 @@
     <xf numFmtId="1" fontId="0" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="15" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="15" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="15" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="15" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="15" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="11" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="15" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="15" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="15" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="15" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="15" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="10" borderId="45" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="12" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="45" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="45" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="45" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="48" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="45" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="45" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1302,10 +1726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27448E1A-C569-4D0E-A2D4-4F122CC6FED9}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="J21" sqref="A1:J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1317,7 +1741,7 @@
     <col min="9" max="9" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -1337,16 +1761,19 @@
         <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="46">
         <v>1</v>
       </c>
@@ -1366,19 +1793,23 @@
         <f t="shared" ref="F2:F21" si="0">E2*D2</f>
         <v>5.56</v>
       </c>
-      <c r="G2" s="113">
+      <c r="G2" s="133">
+        <f>SUM(F2:F3)</f>
+        <v>20.02</v>
+      </c>
+      <c r="H2" s="110">
         <f>SUM(F2:F4)</f>
         <v>48.94</v>
       </c>
-      <c r="H2" s="119">
-        <v>2</v>
-      </c>
-      <c r="I2" s="116">
-        <f>G2/H2</f>
+      <c r="I2" s="113">
+        <v>2</v>
+      </c>
+      <c r="J2" s="127">
+        <f>H2/I2</f>
         <v>24.47</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="49">
         <v>1</v>
       </c>
@@ -1398,11 +1829,12 @@
         <f t="shared" si="0"/>
         <v>14.46</v>
       </c>
-      <c r="G3" s="114"/>
-      <c r="H3" s="120"/>
-      <c r="I3" s="117"/>
-    </row>
-    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G3" s="134"/>
+      <c r="H3" s="111"/>
+      <c r="I3" s="114"/>
+      <c r="J3" s="128"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="50">
         <v>1</v>
       </c>
@@ -1422,11 +1854,15 @@
         <f t="shared" si="0"/>
         <v>28.92</v>
       </c>
-      <c r="G4" s="115"/>
-      <c r="H4" s="121"/>
-      <c r="I4" s="118"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G4" s="8">
+        <f>SUM(F4)</f>
+        <v>28.92</v>
+      </c>
+      <c r="H4" s="112"/>
+      <c r="I4" s="115"/>
+      <c r="J4" s="129"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="75">
         <v>2</v>
       </c>
@@ -1446,19 +1882,23 @@
         <f t="shared" si="0"/>
         <v>2.62</v>
       </c>
-      <c r="G5" s="113">
+      <c r="G5" s="133">
+        <f>SUM(F5:F8)</f>
+        <v>31.409999999999997</v>
+      </c>
+      <c r="H5" s="110">
         <f>SUM(F5:F9)</f>
         <v>64.77</v>
       </c>
-      <c r="H5" s="119">
-        <v>2</v>
-      </c>
-      <c r="I5" s="110">
-        <f>G5/H5</f>
+      <c r="I5" s="113">
+        <v>2</v>
+      </c>
+      <c r="J5" s="130">
+        <f>H5/I5</f>
         <v>32.384999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="75">
         <v>2</v>
       </c>
@@ -1478,11 +1918,12 @@
         <f t="shared" si="0"/>
         <v>2.62</v>
       </c>
-      <c r="G6" s="114"/>
-      <c r="H6" s="120"/>
-      <c r="I6" s="111"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G6" s="135"/>
+      <c r="H6" s="111"/>
+      <c r="I6" s="114"/>
+      <c r="J6" s="131"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="75">
         <v>2</v>
       </c>
@@ -1502,11 +1943,12 @@
         <f t="shared" si="0"/>
         <v>3.93</v>
       </c>
-      <c r="G7" s="114"/>
-      <c r="H7" s="120"/>
-      <c r="I7" s="111"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G7" s="135"/>
+      <c r="H7" s="111"/>
+      <c r="I7" s="114"/>
+      <c r="J7" s="131"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="76">
         <v>2</v>
       </c>
@@ -1526,11 +1968,12 @@
         <f t="shared" si="0"/>
         <v>22.24</v>
       </c>
-      <c r="G8" s="114"/>
-      <c r="H8" s="120"/>
-      <c r="I8" s="111"/>
-    </row>
-    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G8" s="134"/>
+      <c r="H8" s="111"/>
+      <c r="I8" s="114"/>
+      <c r="J8" s="131"/>
+    </row>
+    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="77">
         <v>2</v>
       </c>
@@ -1550,11 +1993,15 @@
         <f t="shared" si="0"/>
         <v>33.36</v>
       </c>
-      <c r="G9" s="115"/>
-      <c r="H9" s="121"/>
-      <c r="I9" s="112"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G9" s="5">
+        <f>SUM(F9)</f>
+        <v>33.36</v>
+      </c>
+      <c r="H9" s="112"/>
+      <c r="I9" s="115"/>
+      <c r="J9" s="132"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="55">
         <v>3</v>
       </c>
@@ -1574,19 +2021,23 @@
         <f t="shared" si="0"/>
         <v>3.93</v>
       </c>
-      <c r="G10" s="113">
+      <c r="G10" s="133">
+        <f>SUM(F10:F12)</f>
+        <v>70.649999999999991</v>
+      </c>
+      <c r="H10" s="110">
         <f>SUM(F10:F13)</f>
         <v>142.94999999999999</v>
       </c>
-      <c r="H10" s="119">
-        <v>2</v>
-      </c>
-      <c r="I10" s="110">
-        <f>G10/H10</f>
+      <c r="I10" s="113">
+        <v>2</v>
+      </c>
+      <c r="J10" s="130">
+        <f>H10/I10</f>
         <v>71.474999999999994</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="57">
         <v>3</v>
       </c>
@@ -1606,11 +2057,12 @@
         <f t="shared" si="0"/>
         <v>27.799999999999997</v>
       </c>
-      <c r="G11" s="114"/>
-      <c r="H11" s="120"/>
-      <c r="I11" s="111"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G11" s="135"/>
+      <c r="H11" s="111"/>
+      <c r="I11" s="114"/>
+      <c r="J11" s="131"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="58">
         <v>3</v>
       </c>
@@ -1630,11 +2082,12 @@
         <f t="shared" si="0"/>
         <v>38.919999999999995</v>
       </c>
-      <c r="G12" s="114"/>
-      <c r="H12" s="120"/>
-      <c r="I12" s="111"/>
-    </row>
-    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G12" s="134"/>
+      <c r="H12" s="111"/>
+      <c r="I12" s="114"/>
+      <c r="J12" s="131"/>
+    </row>
+    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="59">
         <v>3</v>
       </c>
@@ -1654,11 +2107,15 @@
         <f t="shared" si="0"/>
         <v>72.300000000000011</v>
       </c>
-      <c r="G13" s="115"/>
-      <c r="H13" s="121"/>
-      <c r="I13" s="112"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G13" s="6">
+        <f>SUM(F13)</f>
+        <v>72.300000000000011</v>
+      </c>
+      <c r="H13" s="112"/>
+      <c r="I13" s="115"/>
+      <c r="J13" s="132"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="78">
         <v>4</v>
       </c>
@@ -1678,19 +2135,23 @@
         <f t="shared" si="0"/>
         <v>1.31</v>
       </c>
-      <c r="G14" s="113">
+      <c r="G14" s="133">
+        <f>SUM(F14:F15)</f>
+        <v>12.43</v>
+      </c>
+      <c r="H14" s="110">
         <f>SUM(F14:F17)</f>
         <v>20.97</v>
       </c>
-      <c r="H14" s="119">
-        <v>2</v>
-      </c>
-      <c r="I14" s="110">
-        <f>G14/H14</f>
+      <c r="I14" s="113">
+        <v>2</v>
+      </c>
+      <c r="J14" s="130">
+        <f>H14/I14</f>
         <v>10.484999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="79">
         <v>4</v>
       </c>
@@ -1710,11 +2171,12 @@
         <f t="shared" si="0"/>
         <v>11.12</v>
       </c>
-      <c r="G15" s="114"/>
-      <c r="H15" s="120"/>
-      <c r="I15" s="111"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G15" s="134"/>
+      <c r="H15" s="111"/>
+      <c r="I15" s="114"/>
+      <c r="J15" s="131"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="80">
         <v>4</v>
       </c>
@@ -1734,11 +2196,15 @@
         <f t="shared" si="0"/>
         <v>1.31</v>
       </c>
-      <c r="G16" s="114"/>
-      <c r="H16" s="120"/>
-      <c r="I16" s="111"/>
-    </row>
-    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G16" s="136">
+        <f>SUM(F16:F17)</f>
+        <v>8.5400000000000009</v>
+      </c>
+      <c r="H16" s="111"/>
+      <c r="I16" s="114"/>
+      <c r="J16" s="131"/>
+    </row>
+    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="81">
         <v>4</v>
       </c>
@@ -1758,11 +2224,12 @@
         <f t="shared" si="0"/>
         <v>7.23</v>
       </c>
-      <c r="G17" s="115"/>
-      <c r="H17" s="121"/>
-      <c r="I17" s="112"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G17" s="137"/>
+      <c r="H17" s="112"/>
+      <c r="I17" s="115"/>
+      <c r="J17" s="132"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="65">
         <v>5</v>
       </c>
@@ -1782,19 +2249,23 @@
         <f t="shared" si="0"/>
         <v>1.31</v>
       </c>
-      <c r="G18" s="113">
+      <c r="G18" s="133">
+        <f>SUM(F18:F19)</f>
+        <v>12.43</v>
+      </c>
+      <c r="H18" s="110">
         <f>SUM(F18:F20)</f>
         <v>20.83</v>
       </c>
-      <c r="H18" s="119">
-        <v>2</v>
-      </c>
-      <c r="I18" s="110">
-        <f>G18/H18</f>
+      <c r="I18" s="113">
+        <v>2</v>
+      </c>
+      <c r="J18" s="130">
+        <f>H18/I18</f>
         <v>10.414999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="67">
         <v>5</v>
       </c>
@@ -1814,11 +2285,12 @@
         <f t="shared" si="0"/>
         <v>11.12</v>
       </c>
-      <c r="G19" s="114"/>
-      <c r="H19" s="120"/>
-      <c r="I19" s="111"/>
-    </row>
-    <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G19" s="134"/>
+      <c r="H19" s="111"/>
+      <c r="I19" s="114"/>
+      <c r="J19" s="131"/>
+    </row>
+    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="68">
         <v>5</v>
       </c>
@@ -1838,11 +2310,15 @@
         <f t="shared" si="0"/>
         <v>8.4</v>
       </c>
-      <c r="G20" s="115"/>
-      <c r="H20" s="121"/>
-      <c r="I20" s="112"/>
-    </row>
-    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G20" s="6">
+        <f>SUM(F20)</f>
+        <v>8.4</v>
+      </c>
+      <c r="H20" s="112"/>
+      <c r="I20" s="115"/>
+      <c r="J20" s="132"/>
+    </row>
+    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="71">
         <v>6</v>
       </c>
@@ -1862,32 +2338,40 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="G21" s="108">
+      <c r="G21" s="9">
         <f>SUM(F21)</f>
         <v>21</v>
       </c>
-      <c r="H21" s="109">
-        <v>1</v>
-      </c>
-      <c r="I21" s="74">
-        <f t="shared" ref="I21:I22" si="1">G21/H21</f>
+      <c r="H21" s="108">
+        <f>SUM(F21)</f>
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I21" s="109">
+        <v>1</v>
+      </c>
+      <c r="J21" s="74">
+        <f t="shared" ref="J21:J22" si="1">H21/I21</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F22" s="10">
         <f>SUM(F2:F21)</f>
         <v>319.45999999999998</v>
       </c>
-      <c r="G22" s="11">
-        <f>SUM(G2:G21)</f>
+      <c r="G22" s="10">
+        <f>SUM(F2:F21)</f>
         <v>319.45999999999998</v>
       </c>
       <c r="H22" s="11">
+        <f>SUM(F2:F21)</f>
+        <v>319.45999999999998</v>
+      </c>
+      <c r="I22" s="11">
         <v>11</v>
       </c>
-      <c r="I22" s="12">
-        <f t="shared" si="1"/>
+      <c r="J22" s="12">
+        <f>H22/I22</f>
         <v>29.041818181818179</v>
       </c>
     </row>
@@ -1898,28 +2382,579 @@
     <sortCondition ref="C2:C21"/>
     <sortCondition ref="D2:D21"/>
   </sortState>
-  <mergeCells count="15">
+  <mergeCells count="21">
+    <mergeCell ref="G5:G8"/>
+    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="J2:J4"/>
+    <mergeCell ref="J5:J9"/>
+    <mergeCell ref="J10:J13"/>
+    <mergeCell ref="J14:J17"/>
+    <mergeCell ref="J18:J20"/>
     <mergeCell ref="I14:I17"/>
     <mergeCell ref="I18:I20"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="G5:G9"/>
-    <mergeCell ref="G10:G13"/>
-    <mergeCell ref="G14:G17"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="I5:I9"/>
-    <mergeCell ref="I10:I13"/>
     <mergeCell ref="H2:H4"/>
     <mergeCell ref="H5:H9"/>
     <mergeCell ref="H10:H13"/>
     <mergeCell ref="H14:H17"/>
     <mergeCell ref="H18:H20"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="I5:I9"/>
+    <mergeCell ref="I10:I13"/>
+    <mergeCell ref="G2:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A58B81F8-84E9-4D93-9DFE-6EC1C4A58AE4}">
+  <dimension ref="A1:G21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="143">
+        <v>5</v>
+      </c>
+      <c r="B2" s="144">
+        <v>2</v>
+      </c>
+      <c r="C2" s="144" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="144">
+        <v>2</v>
+      </c>
+      <c r="E2" s="145">
+        <v>4.2</v>
+      </c>
+      <c r="F2" s="146">
+        <f>E2*D2</f>
+        <v>8.4</v>
+      </c>
+      <c r="G2" s="147">
+        <f>SUM(F2)</f>
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="173">
+        <v>4</v>
+      </c>
+      <c r="B3" s="174">
+        <v>2</v>
+      </c>
+      <c r="C3" s="174" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="174">
+        <v>1</v>
+      </c>
+      <c r="E3" s="174">
+        <v>1.31</v>
+      </c>
+      <c r="F3" s="155">
+        <f>E3*D3</f>
+        <v>1.31</v>
+      </c>
+      <c r="G3" s="156">
+        <f>SUM(F3:F4)</f>
+        <v>8.5400000000000009</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="175">
+        <v>4</v>
+      </c>
+      <c r="B4" s="176">
+        <v>2</v>
+      </c>
+      <c r="C4" s="176" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="176">
+        <v>1</v>
+      </c>
+      <c r="E4" s="177">
+        <v>7.23</v>
+      </c>
+      <c r="F4" s="160">
+        <f>E4*D4</f>
+        <v>7.23</v>
+      </c>
+      <c r="G4" s="161">
+        <f>SUM(F3:F4)</f>
+        <v>8.5400000000000009</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="178">
+        <v>4</v>
+      </c>
+      <c r="B5" s="179">
+        <v>1</v>
+      </c>
+      <c r="C5" s="179" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="179">
+        <v>1</v>
+      </c>
+      <c r="E5" s="179">
+        <v>1.31</v>
+      </c>
+      <c r="F5" s="155">
+        <f>E5*D5</f>
+        <v>1.31</v>
+      </c>
+      <c r="G5" s="156">
+        <f>SUM(F5:F6)</f>
+        <v>12.43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="180">
+        <v>4</v>
+      </c>
+      <c r="B6" s="181">
+        <v>1</v>
+      </c>
+      <c r="C6" s="181" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="181">
+        <v>2</v>
+      </c>
+      <c r="E6" s="182">
+        <v>5.56</v>
+      </c>
+      <c r="F6" s="160">
+        <f>E6*D6</f>
+        <v>11.12</v>
+      </c>
+      <c r="G6" s="161">
+        <f>SUM(F5:F6)</f>
+        <v>12.43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="153">
+        <v>5</v>
+      </c>
+      <c r="B7" s="154">
+        <v>1</v>
+      </c>
+      <c r="C7" s="154" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="154">
+        <v>1</v>
+      </c>
+      <c r="E7" s="154">
+        <v>1.31</v>
+      </c>
+      <c r="F7" s="155">
+        <f>E7*D7</f>
+        <v>1.31</v>
+      </c>
+      <c r="G7" s="156">
+        <f>SUM(F7:F8)</f>
+        <v>12.43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="157">
+        <v>5</v>
+      </c>
+      <c r="B8" s="158">
+        <v>1</v>
+      </c>
+      <c r="C8" s="158" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="158">
+        <v>2</v>
+      </c>
+      <c r="E8" s="159">
+        <v>5.56</v>
+      </c>
+      <c r="F8" s="160">
+        <f>E8*D8</f>
+        <v>11.12</v>
+      </c>
+      <c r="G8" s="161">
+        <f>SUM(F7:F8)</f>
+        <v>12.43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="183">
+        <v>1</v>
+      </c>
+      <c r="B9" s="184">
+        <v>1</v>
+      </c>
+      <c r="C9" s="184" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="184">
+        <v>1</v>
+      </c>
+      <c r="E9" s="185">
+        <v>5.56</v>
+      </c>
+      <c r="F9" s="155">
+        <f>E9*D9</f>
+        <v>5.56</v>
+      </c>
+      <c r="G9" s="156">
+        <f>SUM(F9:F10)</f>
+        <v>20.02</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="186">
+        <v>1</v>
+      </c>
+      <c r="B10" s="187">
+        <v>1</v>
+      </c>
+      <c r="C10" s="187" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="187">
+        <v>2</v>
+      </c>
+      <c r="E10" s="188">
+        <v>7.23</v>
+      </c>
+      <c r="F10" s="160">
+        <f>E10*D10</f>
+        <v>14.46</v>
+      </c>
+      <c r="G10" s="161">
+        <f>SUM(F9:F10)</f>
+        <v>20.02</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="162">
+        <v>6</v>
+      </c>
+      <c r="B11" s="163">
+        <v>6</v>
+      </c>
+      <c r="C11" s="163" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="163">
+        <v>5</v>
+      </c>
+      <c r="E11" s="164">
+        <v>4.2</v>
+      </c>
+      <c r="F11" s="146">
+        <f>E11*D11</f>
+        <v>21</v>
+      </c>
+      <c r="G11" s="147">
+        <f>SUM(F11)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="189">
+        <v>1</v>
+      </c>
+      <c r="B12" s="190">
+        <v>7</v>
+      </c>
+      <c r="C12" s="190" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="190">
+        <v>4</v>
+      </c>
+      <c r="E12" s="191">
+        <v>7.23</v>
+      </c>
+      <c r="F12" s="151">
+        <f>E12*D12</f>
+        <v>28.92</v>
+      </c>
+      <c r="G12" s="152">
+        <f>SUM(F12)</f>
+        <v>28.92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="165">
+        <v>2</v>
+      </c>
+      <c r="B13" s="166">
+        <v>1</v>
+      </c>
+      <c r="C13" s="166" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="166">
+        <v>2</v>
+      </c>
+      <c r="E13" s="166">
+        <v>1.31</v>
+      </c>
+      <c r="F13" s="155">
+        <f>E13*D13</f>
+        <v>2.62</v>
+      </c>
+      <c r="G13" s="156">
+        <f>SUM(F13:F16)</f>
+        <v>31.409999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="149">
+        <v>2</v>
+      </c>
+      <c r="B14" s="140">
+        <v>1</v>
+      </c>
+      <c r="C14" s="140" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="140">
+        <v>2</v>
+      </c>
+      <c r="E14" s="140">
+        <v>1.31</v>
+      </c>
+      <c r="F14" s="139">
+        <f>E14*D14</f>
+        <v>2.62</v>
+      </c>
+      <c r="G14" s="148">
+        <f>SUM(F13:F16)</f>
+        <v>31.409999999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="149">
+        <v>2</v>
+      </c>
+      <c r="B15" s="140">
+        <v>1</v>
+      </c>
+      <c r="C15" s="140" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="140">
+        <v>3</v>
+      </c>
+      <c r="E15" s="140">
+        <v>1.31</v>
+      </c>
+      <c r="F15" s="139">
+        <f>E15*D15</f>
+        <v>3.93</v>
+      </c>
+      <c r="G15" s="148">
+        <f>SUM(F13:F16)</f>
+        <v>31.409999999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="167">
+        <v>2</v>
+      </c>
+      <c r="B16" s="168">
+        <v>1</v>
+      </c>
+      <c r="C16" s="168" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="168">
+        <v>4</v>
+      </c>
+      <c r="E16" s="169">
+        <v>5.56</v>
+      </c>
+      <c r="F16" s="160">
+        <f>E16*D16</f>
+        <v>22.24</v>
+      </c>
+      <c r="G16" s="161">
+        <f>SUM(F13:F16)</f>
+        <v>31.409999999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="170">
+        <v>2</v>
+      </c>
+      <c r="B17" s="171">
+        <v>3</v>
+      </c>
+      <c r="C17" s="171" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="171">
+        <v>6</v>
+      </c>
+      <c r="E17" s="172">
+        <v>5.56</v>
+      </c>
+      <c r="F17" s="151">
+        <f>E17*D17</f>
+        <v>33.36</v>
+      </c>
+      <c r="G17" s="152">
+        <f>SUM(F17)</f>
+        <v>33.36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="192">
+        <v>3</v>
+      </c>
+      <c r="B18" s="193">
+        <v>1</v>
+      </c>
+      <c r="C18" s="193" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="193">
+        <v>3</v>
+      </c>
+      <c r="E18" s="193">
+        <v>1.31</v>
+      </c>
+      <c r="F18" s="155">
+        <f>E18*D18</f>
+        <v>3.93</v>
+      </c>
+      <c r="G18" s="156">
+        <f>SUM(F18:F20)</f>
+        <v>70.649999999999991</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="150">
+        <v>3</v>
+      </c>
+      <c r="B19" s="141">
+        <v>1</v>
+      </c>
+      <c r="C19" s="141" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="141">
+        <v>5</v>
+      </c>
+      <c r="E19" s="142">
+        <v>5.56</v>
+      </c>
+      <c r="F19" s="138">
+        <f>E19*D19</f>
+        <v>27.799999999999997</v>
+      </c>
+      <c r="G19" s="148">
+        <f>SUM(F18:F20)</f>
+        <v>70.649999999999991</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="194">
+        <v>3</v>
+      </c>
+      <c r="B20" s="195">
+        <v>1</v>
+      </c>
+      <c r="C20" s="195" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="195">
+        <v>7</v>
+      </c>
+      <c r="E20" s="196">
+        <v>5.56</v>
+      </c>
+      <c r="F20" s="160">
+        <f>E20*D20</f>
+        <v>38.919999999999995</v>
+      </c>
+      <c r="G20" s="161">
+        <f>SUM(F18:F20)</f>
+        <v>70.649999999999991</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="197">
+        <v>3</v>
+      </c>
+      <c r="B21" s="198">
+        <v>2</v>
+      </c>
+      <c r="C21" s="198" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="198">
+        <v>10</v>
+      </c>
+      <c r="E21" s="199">
+        <v>7.23</v>
+      </c>
+      <c r="F21" s="146">
+        <f>E21*D21</f>
+        <v>72.300000000000011</v>
+      </c>
+      <c r="G21" s="147">
+        <f>SUM(F21)</f>
+        <v>72.300000000000011</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G21">
+    <sortCondition ref="G2:G21"/>
+    <sortCondition ref="A2:A21"/>
+    <sortCondition ref="B2:B21"/>
+    <sortCondition ref="C2:C21"/>
+    <sortCondition ref="D2:D21"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D190C58-97B3-4FCC-8D31-8F1AF72C877A}">
   <dimension ref="A1:F22"/>
   <sheetViews>
@@ -1969,7 +3004,7 @@
       <c r="E2" s="23">
         <v>1.31</v>
       </c>
-      <c r="F2" s="122">
+      <c r="F2" s="116">
         <v>5</v>
       </c>
     </row>
@@ -1989,7 +3024,7 @@
       <c r="E3" s="13">
         <v>1.31</v>
       </c>
-      <c r="F3" s="123"/>
+      <c r="F3" s="117"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="25">
@@ -2007,7 +3042,7 @@
       <c r="E4" s="26">
         <v>1.31</v>
       </c>
-      <c r="F4" s="123"/>
+      <c r="F4" s="117"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="87">
@@ -2025,7 +3060,7 @@
       <c r="E5" s="88">
         <v>1.31</v>
       </c>
-      <c r="F5" s="123"/>
+      <c r="F5" s="117"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="87">
@@ -2043,7 +3078,7 @@
       <c r="E6" s="88">
         <v>1.31</v>
       </c>
-      <c r="F6" s="123"/>
+      <c r="F6" s="117"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="87">
@@ -2061,7 +3096,7 @@
       <c r="E7" s="88">
         <v>1.31</v>
       </c>
-      <c r="F7" s="123"/>
+      <c r="F7" s="117"/>
     </row>
     <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="87">
@@ -2079,7 +3114,7 @@
       <c r="E8" s="88">
         <v>1.31</v>
       </c>
-      <c r="F8" s="124"/>
+      <c r="F8" s="118"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
@@ -2097,7 +3132,7 @@
       <c r="E9" s="94">
         <v>5.56</v>
       </c>
-      <c r="F9" s="125">
+      <c r="F9" s="119">
         <v>6</v>
       </c>
     </row>
@@ -2117,7 +3152,7 @@
       <c r="E10" s="94">
         <v>5.56</v>
       </c>
-      <c r="F10" s="125"/>
+      <c r="F10" s="119"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
@@ -2135,7 +3170,7 @@
       <c r="E11" s="94">
         <v>5.56</v>
       </c>
-      <c r="F11" s="125"/>
+      <c r="F11" s="119"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="28">
@@ -2153,7 +3188,7 @@
       <c r="E12" s="95">
         <v>5.56</v>
       </c>
-      <c r="F12" s="125"/>
+      <c r="F12" s="119"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="31">
@@ -2171,7 +3206,7 @@
       <c r="E13" s="33">
         <v>5.56</v>
       </c>
-      <c r="F13" s="125"/>
+      <c r="F13" s="119"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
@@ -2189,7 +3224,7 @@
       <c r="E14" s="94">
         <v>5.56</v>
       </c>
-      <c r="F14" s="125"/>
+      <c r="F14" s="119"/>
     </row>
     <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
@@ -2207,7 +3242,7 @@
       <c r="E15" s="94">
         <v>5.56</v>
       </c>
-      <c r="F15" s="125"/>
+      <c r="F15" s="119"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="90">
@@ -2225,7 +3260,7 @@
       <c r="E16" s="96">
         <v>7.23</v>
       </c>
-      <c r="F16" s="126">
+      <c r="F16" s="120">
         <v>4</v>
       </c>
     </row>
@@ -2245,7 +3280,7 @@
       <c r="E17" s="96">
         <v>7.23</v>
       </c>
-      <c r="F17" s="125"/>
+      <c r="F17" s="119"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="90">
@@ -2263,7 +3298,7 @@
       <c r="E18" s="96">
         <v>7.23</v>
       </c>
-      <c r="F18" s="125"/>
+      <c r="F18" s="119"/>
     </row>
     <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="90">
@@ -2281,7 +3316,7 @@
       <c r="E19" s="96">
         <v>7.23</v>
       </c>
-      <c r="F19" s="127"/>
+      <c r="F19" s="121"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="92">
@@ -2299,7 +3334,7 @@
       <c r="E20" s="97">
         <v>4.2</v>
       </c>
-      <c r="F20" s="125">
+      <c r="F20" s="119">
         <v>2</v>
       </c>
     </row>
@@ -2319,7 +3354,7 @@
       <c r="E21" s="42">
         <v>4.2</v>
       </c>
-      <c r="F21" s="127"/>
+      <c r="F21" s="121"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F22" s="98"/>
@@ -2341,11 +3376,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{278C7FD2-399F-4D80-8AD7-B7131F055316}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
@@ -2412,7 +3447,7 @@
       <c r="E3" s="24">
         <v>7.23</v>
       </c>
-      <c r="F3" s="128">
+      <c r="F3" s="122">
         <v>2</v>
       </c>
     </row>
@@ -2432,7 +3467,7 @@
       <c r="E4" s="27">
         <v>7.23</v>
       </c>
-      <c r="F4" s="129"/>
+      <c r="F4" s="123"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="28">
@@ -2450,7 +3485,7 @@
       <c r="E5" s="29">
         <v>1.31</v>
       </c>
-      <c r="F5" s="128">
+      <c r="F5" s="122">
         <v>1</v>
       </c>
     </row>
@@ -2470,7 +3505,7 @@
       <c r="E6" s="14">
         <v>1.31</v>
       </c>
-      <c r="F6" s="130"/>
+      <c r="F6" s="124"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="31">
@@ -2488,7 +3523,7 @@
       <c r="E7" s="32">
         <v>1.31</v>
       </c>
-      <c r="F7" s="129"/>
+      <c r="F7" s="123"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="75">
@@ -2506,7 +3541,7 @@
       <c r="E8" s="15">
         <v>5.56</v>
       </c>
-      <c r="F8" s="131">
+      <c r="F8" s="125">
         <v>2</v>
       </c>
     </row>
@@ -2526,7 +3561,7 @@
       <c r="E9" s="15">
         <v>5.56</v>
       </c>
-      <c r="F9" s="132"/>
+      <c r="F9" s="126"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="90">
@@ -2564,7 +3599,7 @@
       <c r="E11" s="100">
         <v>5.56</v>
       </c>
-      <c r="F11" s="131">
+      <c r="F11" s="125">
         <v>1</v>
       </c>
     </row>
@@ -2584,7 +3619,7 @@
       <c r="E12" s="38">
         <v>5.56</v>
       </c>
-      <c r="F12" s="132"/>
+      <c r="F12" s="126"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="57">
@@ -2622,7 +3657,7 @@
       <c r="E14" s="40">
         <v>1.31</v>
       </c>
-      <c r="F14" s="131">
+      <c r="F14" s="125">
         <v>2</v>
       </c>
     </row>
@@ -2642,7 +3677,7 @@
       <c r="E15" s="41">
         <v>1.31</v>
       </c>
-      <c r="F15" s="132"/>
+      <c r="F15" s="126"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="92">

</xml_diff>

<commit_message>
Added all tests for RapGenOps
</commit_message>
<xml_diff>
--- a/UnitTests/RaportGeneratorTestData.xlsx
+++ b/UnitTests/RaportGeneratorTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Użytkownik\source\repos\WindowsFormsApp1\UnitTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60BAEC4-7944-4BCB-877B-4B40A2FB567A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2579FD15-E5B1-4B07-A134-7231868AA3E3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{91592E27-BDF5-4EBE-B96A-BEC0E890A090}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{91592E27-BDF5-4EBE-B96A-BEC0E890A090}"/>
   </bookViews>
   <sheets>
     <sheet name="By cid and rid" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="17">
   <si>
     <t>Chleb</t>
   </si>
@@ -76,6 +76,15 @@
   </si>
   <si>
     <t>ReqSum</t>
+  </si>
+  <si>
+    <t>ProdQuant</t>
+  </si>
+  <si>
+    <t>FullPrice</t>
+  </si>
+  <si>
+    <t>P*Q</t>
   </si>
 </sst>
 </file>
@@ -192,7 +201,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="50">
+  <borders count="52">
     <border>
       <left/>
       <right/>
@@ -811,11 +820,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="200">
+  <cellXfs count="212">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1142,6 +1179,234 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="11" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="10" borderId="45" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="12" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="45" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="45" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="45" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="48" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="45" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="45" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1151,15 +1416,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1193,223 +1449,40 @@
     <xf numFmtId="1" fontId="0" fillId="15" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="11" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="10" borderId="45" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="12" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="45" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="9" borderId="45" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="8" borderId="45" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="48" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="45" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="45" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="7" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="15" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="15" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="15" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1729,7 +1802,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J21" sqref="A1:J21"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1793,18 +1866,18 @@
         <f t="shared" ref="F2:F21" si="0">E2*D2</f>
         <v>5.56</v>
       </c>
-      <c r="G2" s="133">
+      <c r="G2" s="172">
         <f>SUM(F2:F3)</f>
         <v>20.02</v>
       </c>
-      <c r="H2" s="110">
+      <c r="H2" s="186">
         <f>SUM(F2:F4)</f>
         <v>48.94</v>
       </c>
-      <c r="I2" s="113">
-        <v>2</v>
-      </c>
-      <c r="J2" s="127">
+      <c r="I2" s="183">
+        <v>2</v>
+      </c>
+      <c r="J2" s="177">
         <f>H2/I2</f>
         <v>24.47</v>
       </c>
@@ -1829,10 +1902,10 @@
         <f t="shared" si="0"/>
         <v>14.46</v>
       </c>
-      <c r="G3" s="134"/>
-      <c r="H3" s="111"/>
-      <c r="I3" s="114"/>
-      <c r="J3" s="128"/>
+      <c r="G3" s="174"/>
+      <c r="H3" s="187"/>
+      <c r="I3" s="184"/>
+      <c r="J3" s="178"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="50">
@@ -1858,9 +1931,9 @@
         <f>SUM(F4)</f>
         <v>28.92</v>
       </c>
-      <c r="H4" s="112"/>
-      <c r="I4" s="115"/>
-      <c r="J4" s="129"/>
+      <c r="H4" s="188"/>
+      <c r="I4" s="185"/>
+      <c r="J4" s="179"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="75">
@@ -1882,18 +1955,18 @@
         <f t="shared" si="0"/>
         <v>2.62</v>
       </c>
-      <c r="G5" s="133">
+      <c r="G5" s="172">
         <f>SUM(F5:F8)</f>
         <v>31.409999999999997</v>
       </c>
-      <c r="H5" s="110">
+      <c r="H5" s="186">
         <f>SUM(F5:F9)</f>
         <v>64.77</v>
       </c>
-      <c r="I5" s="113">
-        <v>2</v>
-      </c>
-      <c r="J5" s="130">
+      <c r="I5" s="183">
+        <v>2</v>
+      </c>
+      <c r="J5" s="180">
         <f>H5/I5</f>
         <v>32.384999999999998</v>
       </c>
@@ -1918,10 +1991,10 @@
         <f t="shared" si="0"/>
         <v>2.62</v>
       </c>
-      <c r="G6" s="135"/>
-      <c r="H6" s="111"/>
-      <c r="I6" s="114"/>
-      <c r="J6" s="131"/>
+      <c r="G6" s="173"/>
+      <c r="H6" s="187"/>
+      <c r="I6" s="184"/>
+      <c r="J6" s="181"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="75">
@@ -1943,10 +2016,10 @@
         <f t="shared" si="0"/>
         <v>3.93</v>
       </c>
-      <c r="G7" s="135"/>
-      <c r="H7" s="111"/>
-      <c r="I7" s="114"/>
-      <c r="J7" s="131"/>
+      <c r="G7" s="173"/>
+      <c r="H7" s="187"/>
+      <c r="I7" s="184"/>
+      <c r="J7" s="181"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="76">
@@ -1968,10 +2041,10 @@
         <f t="shared" si="0"/>
         <v>22.24</v>
       </c>
-      <c r="G8" s="134"/>
-      <c r="H8" s="111"/>
-      <c r="I8" s="114"/>
-      <c r="J8" s="131"/>
+      <c r="G8" s="174"/>
+      <c r="H8" s="187"/>
+      <c r="I8" s="184"/>
+      <c r="J8" s="181"/>
     </row>
     <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="77">
@@ -1997,9 +2070,9 @@
         <f>SUM(F9)</f>
         <v>33.36</v>
       </c>
-      <c r="H9" s="112"/>
-      <c r="I9" s="115"/>
-      <c r="J9" s="132"/>
+      <c r="H9" s="188"/>
+      <c r="I9" s="185"/>
+      <c r="J9" s="182"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="55">
@@ -2021,18 +2094,18 @@
         <f t="shared" si="0"/>
         <v>3.93</v>
       </c>
-      <c r="G10" s="133">
+      <c r="G10" s="172">
         <f>SUM(F10:F12)</f>
         <v>70.649999999999991</v>
       </c>
-      <c r="H10" s="110">
+      <c r="H10" s="186">
         <f>SUM(F10:F13)</f>
         <v>142.94999999999999</v>
       </c>
-      <c r="I10" s="113">
-        <v>2</v>
-      </c>
-      <c r="J10" s="130">
+      <c r="I10" s="183">
+        <v>2</v>
+      </c>
+      <c r="J10" s="180">
         <f>H10/I10</f>
         <v>71.474999999999994</v>
       </c>
@@ -2057,10 +2130,10 @@
         <f t="shared" si="0"/>
         <v>27.799999999999997</v>
       </c>
-      <c r="G11" s="135"/>
-      <c r="H11" s="111"/>
-      <c r="I11" s="114"/>
-      <c r="J11" s="131"/>
+      <c r="G11" s="173"/>
+      <c r="H11" s="187"/>
+      <c r="I11" s="184"/>
+      <c r="J11" s="181"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="58">
@@ -2082,10 +2155,10 @@
         <f t="shared" si="0"/>
         <v>38.919999999999995</v>
       </c>
-      <c r="G12" s="134"/>
-      <c r="H12" s="111"/>
-      <c r="I12" s="114"/>
-      <c r="J12" s="131"/>
+      <c r="G12" s="174"/>
+      <c r="H12" s="187"/>
+      <c r="I12" s="184"/>
+      <c r="J12" s="181"/>
     </row>
     <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="59">
@@ -2111,9 +2184,9 @@
         <f>SUM(F13)</f>
         <v>72.300000000000011</v>
       </c>
-      <c r="H13" s="112"/>
-      <c r="I13" s="115"/>
-      <c r="J13" s="132"/>
+      <c r="H13" s="188"/>
+      <c r="I13" s="185"/>
+      <c r="J13" s="182"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="78">
@@ -2135,18 +2208,18 @@
         <f t="shared" si="0"/>
         <v>1.31</v>
       </c>
-      <c r="G14" s="133">
+      <c r="G14" s="172">
         <f>SUM(F14:F15)</f>
         <v>12.43</v>
       </c>
-      <c r="H14" s="110">
+      <c r="H14" s="186">
         <f>SUM(F14:F17)</f>
         <v>20.97</v>
       </c>
-      <c r="I14" s="113">
-        <v>2</v>
-      </c>
-      <c r="J14" s="130">
+      <c r="I14" s="183">
+        <v>2</v>
+      </c>
+      <c r="J14" s="180">
         <f>H14/I14</f>
         <v>10.484999999999999</v>
       </c>
@@ -2171,10 +2244,10 @@
         <f t="shared" si="0"/>
         <v>11.12</v>
       </c>
-      <c r="G15" s="134"/>
-      <c r="H15" s="111"/>
-      <c r="I15" s="114"/>
-      <c r="J15" s="131"/>
+      <c r="G15" s="174"/>
+      <c r="H15" s="187"/>
+      <c r="I15" s="184"/>
+      <c r="J15" s="181"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="80">
@@ -2196,13 +2269,13 @@
         <f t="shared" si="0"/>
         <v>1.31</v>
       </c>
-      <c r="G16" s="136">
+      <c r="G16" s="175">
         <f>SUM(F16:F17)</f>
         <v>8.5400000000000009</v>
       </c>
-      <c r="H16" s="111"/>
-      <c r="I16" s="114"/>
-      <c r="J16" s="131"/>
+      <c r="H16" s="187"/>
+      <c r="I16" s="184"/>
+      <c r="J16" s="181"/>
     </row>
     <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="81">
@@ -2224,10 +2297,10 @@
         <f t="shared" si="0"/>
         <v>7.23</v>
       </c>
-      <c r="G17" s="137"/>
-      <c r="H17" s="112"/>
-      <c r="I17" s="115"/>
-      <c r="J17" s="132"/>
+      <c r="G17" s="176"/>
+      <c r="H17" s="188"/>
+      <c r="I17" s="185"/>
+      <c r="J17" s="182"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="65">
@@ -2249,18 +2322,18 @@
         <f t="shared" si="0"/>
         <v>1.31</v>
       </c>
-      <c r="G18" s="133">
+      <c r="G18" s="172">
         <f>SUM(F18:F19)</f>
         <v>12.43</v>
       </c>
-      <c r="H18" s="110">
+      <c r="H18" s="186">
         <f>SUM(F18:F20)</f>
         <v>20.83</v>
       </c>
-      <c r="I18" s="113">
-        <v>2</v>
-      </c>
-      <c r="J18" s="130">
+      <c r="I18" s="183">
+        <v>2</v>
+      </c>
+      <c r="J18" s="180">
         <f>H18/I18</f>
         <v>10.414999999999999</v>
       </c>
@@ -2285,10 +2358,10 @@
         <f t="shared" si="0"/>
         <v>11.12</v>
       </c>
-      <c r="G19" s="134"/>
-      <c r="H19" s="111"/>
-      <c r="I19" s="114"/>
-      <c r="J19" s="131"/>
+      <c r="G19" s="174"/>
+      <c r="H19" s="187"/>
+      <c r="I19" s="184"/>
+      <c r="J19" s="181"/>
     </row>
     <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="68">
@@ -2314,9 +2387,9 @@
         <f>SUM(F20)</f>
         <v>8.4</v>
       </c>
-      <c r="H20" s="112"/>
-      <c r="I20" s="115"/>
-      <c r="J20" s="132"/>
+      <c r="H20" s="188"/>
+      <c r="I20" s="185"/>
+      <c r="J20" s="182"/>
     </row>
     <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="71">
@@ -2350,7 +2423,7 @@
         <v>1</v>
       </c>
       <c r="J21" s="74">
-        <f t="shared" ref="J21:J22" si="1">H21/I21</f>
+        <f t="shared" ref="J21" si="1">H21/I21</f>
         <v>21</v>
       </c>
     </row>
@@ -2383,16 +2456,7 @@
     <sortCondition ref="D2:D21"/>
   </sortState>
   <mergeCells count="21">
-    <mergeCell ref="G5:G8"/>
-    <mergeCell ref="G10:G12"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="J2:J4"/>
-    <mergeCell ref="J5:J9"/>
-    <mergeCell ref="J10:J13"/>
-    <mergeCell ref="J14:J17"/>
-    <mergeCell ref="J18:J20"/>
+    <mergeCell ref="G2:G3"/>
     <mergeCell ref="I14:I17"/>
     <mergeCell ref="I18:I20"/>
     <mergeCell ref="H2:H4"/>
@@ -2403,7 +2467,16 @@
     <mergeCell ref="I2:I4"/>
     <mergeCell ref="I5:I9"/>
     <mergeCell ref="I10:I13"/>
-    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="J2:J4"/>
+    <mergeCell ref="J5:J9"/>
+    <mergeCell ref="J10:J13"/>
+    <mergeCell ref="J14:J17"/>
+    <mergeCell ref="J18:J20"/>
+    <mergeCell ref="G5:G8"/>
+    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="G18:G19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2413,7 +2486,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A58B81F8-84E9-4D93-9DFE-6EC1C4A58AE4}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
@@ -2443,501 +2516,501 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="143">
+      <c r="A2" s="115">
         <v>5</v>
       </c>
-      <c r="B2" s="144">
-        <v>2</v>
-      </c>
-      <c r="C2" s="144" t="s">
+      <c r="B2" s="116">
+        <v>2</v>
+      </c>
+      <c r="C2" s="116" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="144">
-        <v>2</v>
-      </c>
-      <c r="E2" s="145">
+      <c r="D2" s="116">
+        <v>2</v>
+      </c>
+      <c r="E2" s="117">
         <v>4.2</v>
       </c>
-      <c r="F2" s="146">
-        <f>E2*D2</f>
+      <c r="F2" s="118">
+        <f t="shared" ref="F2:F21" si="0">E2*D2</f>
         <v>8.4</v>
       </c>
-      <c r="G2" s="147">
+      <c r="G2" s="119">
         <f>SUM(F2)</f>
         <v>8.4</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="173">
+      <c r="A3" s="145">
         <v>4</v>
       </c>
-      <c r="B3" s="174">
-        <v>2</v>
-      </c>
-      <c r="C3" s="174" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="174">
-        <v>1</v>
-      </c>
-      <c r="E3" s="174">
+      <c r="B3" s="146">
+        <v>2</v>
+      </c>
+      <c r="C3" s="146" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="146">
+        <v>1</v>
+      </c>
+      <c r="E3" s="146">
         <v>1.31</v>
       </c>
-      <c r="F3" s="155">
-        <f>E3*D3</f>
+      <c r="F3" s="127">
+        <f t="shared" si="0"/>
         <v>1.31</v>
       </c>
-      <c r="G3" s="156">
+      <c r="G3" s="128">
         <f>SUM(F3:F4)</f>
         <v>8.5400000000000009</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="175">
+      <c r="A4" s="147">
         <v>4</v>
       </c>
-      <c r="B4" s="176">
-        <v>2</v>
-      </c>
-      <c r="C4" s="176" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="176">
-        <v>1</v>
-      </c>
-      <c r="E4" s="177">
+      <c r="B4" s="148">
+        <v>2</v>
+      </c>
+      <c r="C4" s="148" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="148">
+        <v>1</v>
+      </c>
+      <c r="E4" s="149">
         <v>7.23</v>
       </c>
-      <c r="F4" s="160">
-        <f>E4*D4</f>
+      <c r="F4" s="132">
+        <f t="shared" si="0"/>
         <v>7.23</v>
       </c>
-      <c r="G4" s="161">
+      <c r="G4" s="133">
         <f>SUM(F3:F4)</f>
         <v>8.5400000000000009</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="178">
+      <c r="A5" s="150">
         <v>4</v>
       </c>
-      <c r="B5" s="179">
-        <v>1</v>
-      </c>
-      <c r="C5" s="179" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="179">
-        <v>1</v>
-      </c>
-      <c r="E5" s="179">
+      <c r="B5" s="151">
+        <v>1</v>
+      </c>
+      <c r="C5" s="151" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="151">
+        <v>1</v>
+      </c>
+      <c r="E5" s="151">
         <v>1.31</v>
       </c>
-      <c r="F5" s="155">
-        <f>E5*D5</f>
+      <c r="F5" s="127">
+        <f t="shared" si="0"/>
         <v>1.31</v>
       </c>
-      <c r="G5" s="156">
+      <c r="G5" s="128">
         <f>SUM(F5:F6)</f>
         <v>12.43</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="180">
+      <c r="A6" s="152">
         <v>4</v>
       </c>
-      <c r="B6" s="181">
-        <v>1</v>
-      </c>
-      <c r="C6" s="181" t="s">
+      <c r="B6" s="153">
+        <v>1</v>
+      </c>
+      <c r="C6" s="153" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="181">
-        <v>2</v>
-      </c>
-      <c r="E6" s="182">
+      <c r="D6" s="153">
+        <v>2</v>
+      </c>
+      <c r="E6" s="154">
         <v>5.56</v>
       </c>
-      <c r="F6" s="160">
-        <f>E6*D6</f>
+      <c r="F6" s="132">
+        <f t="shared" si="0"/>
         <v>11.12</v>
       </c>
-      <c r="G6" s="161">
+      <c r="G6" s="133">
         <f>SUM(F5:F6)</f>
         <v>12.43</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="153">
+      <c r="A7" s="125">
         <v>5</v>
       </c>
-      <c r="B7" s="154">
-        <v>1</v>
-      </c>
-      <c r="C7" s="154" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="154">
-        <v>1</v>
-      </c>
-      <c r="E7" s="154">
+      <c r="B7" s="126">
+        <v>1</v>
+      </c>
+      <c r="C7" s="126" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="126">
+        <v>1</v>
+      </c>
+      <c r="E7" s="126">
         <v>1.31</v>
       </c>
-      <c r="F7" s="155">
-        <f>E7*D7</f>
+      <c r="F7" s="127">
+        <f t="shared" si="0"/>
         <v>1.31</v>
       </c>
-      <c r="G7" s="156">
+      <c r="G7" s="128">
         <f>SUM(F7:F8)</f>
         <v>12.43</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="157">
+      <c r="A8" s="129">
         <v>5</v>
       </c>
-      <c r="B8" s="158">
-        <v>1</v>
-      </c>
-      <c r="C8" s="158" t="s">
+      <c r="B8" s="130">
+        <v>1</v>
+      </c>
+      <c r="C8" s="130" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="158">
-        <v>2</v>
-      </c>
-      <c r="E8" s="159">
+      <c r="D8" s="130">
+        <v>2</v>
+      </c>
+      <c r="E8" s="131">
         <v>5.56</v>
       </c>
-      <c r="F8" s="160">
-        <f>E8*D8</f>
+      <c r="F8" s="132">
+        <f t="shared" si="0"/>
         <v>11.12</v>
       </c>
-      <c r="G8" s="161">
+      <c r="G8" s="133">
         <f>SUM(F7:F8)</f>
         <v>12.43</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="183">
-        <v>1</v>
-      </c>
-      <c r="B9" s="184">
-        <v>1</v>
-      </c>
-      <c r="C9" s="184" t="s">
+      <c r="A9" s="155">
+        <v>1</v>
+      </c>
+      <c r="B9" s="156">
+        <v>1</v>
+      </c>
+      <c r="C9" s="156" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="184">
-        <v>1</v>
-      </c>
-      <c r="E9" s="185">
+      <c r="D9" s="156">
+        <v>1</v>
+      </c>
+      <c r="E9" s="157">
         <v>5.56</v>
       </c>
-      <c r="F9" s="155">
-        <f>E9*D9</f>
+      <c r="F9" s="127">
+        <f t="shared" si="0"/>
         <v>5.56</v>
       </c>
-      <c r="G9" s="156">
+      <c r="G9" s="128">
         <f>SUM(F9:F10)</f>
         <v>20.02</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="186">
-        <v>1</v>
-      </c>
-      <c r="B10" s="187">
-        <v>1</v>
-      </c>
-      <c r="C10" s="187" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="187">
-        <v>2</v>
-      </c>
-      <c r="E10" s="188">
+      <c r="A10" s="158">
+        <v>1</v>
+      </c>
+      <c r="B10" s="159">
+        <v>1</v>
+      </c>
+      <c r="C10" s="159" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="159">
+        <v>2</v>
+      </c>
+      <c r="E10" s="160">
         <v>7.23</v>
       </c>
-      <c r="F10" s="160">
-        <f>E10*D10</f>
+      <c r="F10" s="132">
+        <f t="shared" si="0"/>
         <v>14.46</v>
       </c>
-      <c r="G10" s="161">
+      <c r="G10" s="133">
         <f>SUM(F9:F10)</f>
         <v>20.02</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="162">
+      <c r="A11" s="134">
         <v>6</v>
       </c>
-      <c r="B11" s="163">
+      <c r="B11" s="135">
         <v>6</v>
       </c>
-      <c r="C11" s="163" t="s">
+      <c r="C11" s="135" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="163">
+      <c r="D11" s="135">
         <v>5</v>
       </c>
-      <c r="E11" s="164">
+      <c r="E11" s="136">
         <v>4.2</v>
       </c>
-      <c r="F11" s="146">
-        <f>E11*D11</f>
+      <c r="F11" s="118">
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="G11" s="147">
+      <c r="G11" s="119">
         <f>SUM(F11)</f>
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="189">
-        <v>1</v>
-      </c>
-      <c r="B12" s="190">
+      <c r="A12" s="161">
+        <v>1</v>
+      </c>
+      <c r="B12" s="162">
         <v>7</v>
       </c>
-      <c r="C12" s="190" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="190">
+      <c r="C12" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="162">
         <v>4</v>
       </c>
-      <c r="E12" s="191">
+      <c r="E12" s="163">
         <v>7.23</v>
       </c>
-      <c r="F12" s="151">
-        <f>E12*D12</f>
+      <c r="F12" s="123">
+        <f t="shared" si="0"/>
         <v>28.92</v>
       </c>
-      <c r="G12" s="152">
+      <c r="G12" s="124">
         <f>SUM(F12)</f>
         <v>28.92</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="165">
-        <v>2</v>
-      </c>
-      <c r="B13" s="166">
-        <v>1</v>
-      </c>
-      <c r="C13" s="166" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="166">
-        <v>2</v>
-      </c>
-      <c r="E13" s="166">
+      <c r="A13" s="137">
+        <v>2</v>
+      </c>
+      <c r="B13" s="138">
+        <v>1</v>
+      </c>
+      <c r="C13" s="138" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="138">
+        <v>2</v>
+      </c>
+      <c r="E13" s="138">
         <v>1.31</v>
       </c>
-      <c r="F13" s="155">
-        <f>E13*D13</f>
+      <c r="F13" s="127">
+        <f t="shared" si="0"/>
         <v>2.62</v>
       </c>
-      <c r="G13" s="156">
+      <c r="G13" s="128">
         <f>SUM(F13:F16)</f>
         <v>31.409999999999997</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="149">
-        <v>2</v>
-      </c>
-      <c r="B14" s="140">
-        <v>1</v>
-      </c>
-      <c r="C14" s="140" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="140">
-        <v>2</v>
-      </c>
-      <c r="E14" s="140">
+      <c r="A14" s="121">
+        <v>2</v>
+      </c>
+      <c r="B14" s="112">
+        <v>1</v>
+      </c>
+      <c r="C14" s="112" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="112">
+        <v>2</v>
+      </c>
+      <c r="E14" s="112">
         <v>1.31</v>
       </c>
-      <c r="F14" s="139">
-        <f>E14*D14</f>
+      <c r="F14" s="111">
+        <f t="shared" si="0"/>
         <v>2.62</v>
       </c>
-      <c r="G14" s="148">
+      <c r="G14" s="120">
         <f>SUM(F13:F16)</f>
         <v>31.409999999999997</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="149">
-        <v>2</v>
-      </c>
-      <c r="B15" s="140">
-        <v>1</v>
-      </c>
-      <c r="C15" s="140" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" s="140">
+      <c r="A15" s="121">
+        <v>2</v>
+      </c>
+      <c r="B15" s="112">
+        <v>1</v>
+      </c>
+      <c r="C15" s="112" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="112">
         <v>3</v>
       </c>
-      <c r="E15" s="140">
+      <c r="E15" s="112">
         <v>1.31</v>
       </c>
-      <c r="F15" s="139">
-        <f>E15*D15</f>
+      <c r="F15" s="111">
+        <f t="shared" si="0"/>
         <v>3.93</v>
       </c>
-      <c r="G15" s="148">
+      <c r="G15" s="120">
         <f>SUM(F13:F16)</f>
         <v>31.409999999999997</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="167">
-        <v>2</v>
-      </c>
-      <c r="B16" s="168">
-        <v>1</v>
-      </c>
-      <c r="C16" s="168" t="s">
+      <c r="A16" s="139">
+        <v>2</v>
+      </c>
+      <c r="B16" s="140">
+        <v>1</v>
+      </c>
+      <c r="C16" s="140" t="s">
         <v>0</v>
       </c>
-      <c r="D16" s="168">
+      <c r="D16" s="140">
         <v>4</v>
       </c>
-      <c r="E16" s="169">
+      <c r="E16" s="141">
         <v>5.56</v>
       </c>
-      <c r="F16" s="160">
-        <f>E16*D16</f>
+      <c r="F16" s="132">
+        <f t="shared" si="0"/>
         <v>22.24</v>
       </c>
-      <c r="G16" s="161">
+      <c r="G16" s="133">
         <f>SUM(F13:F16)</f>
         <v>31.409999999999997</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="170">
-        <v>2</v>
-      </c>
-      <c r="B17" s="171">
+      <c r="A17" s="142">
+        <v>2</v>
+      </c>
+      <c r="B17" s="143">
         <v>3</v>
       </c>
-      <c r="C17" s="171" t="s">
+      <c r="C17" s="143" t="s">
         <v>0</v>
       </c>
-      <c r="D17" s="171">
+      <c r="D17" s="143">
         <v>6</v>
       </c>
-      <c r="E17" s="172">
+      <c r="E17" s="144">
         <v>5.56</v>
       </c>
-      <c r="F17" s="151">
-        <f>E17*D17</f>
+      <c r="F17" s="123">
+        <f t="shared" si="0"/>
         <v>33.36</v>
       </c>
-      <c r="G17" s="152">
+      <c r="G17" s="124">
         <f>SUM(F17)</f>
         <v>33.36</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="192">
+      <c r="A18" s="164">
         <v>3</v>
       </c>
-      <c r="B18" s="193">
-        <v>1</v>
-      </c>
-      <c r="C18" s="193" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="193">
+      <c r="B18" s="165">
+        <v>1</v>
+      </c>
+      <c r="C18" s="165" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="165">
         <v>3</v>
       </c>
-      <c r="E18" s="193">
+      <c r="E18" s="165">
         <v>1.31</v>
       </c>
-      <c r="F18" s="155">
-        <f>E18*D18</f>
+      <c r="F18" s="127">
+        <f t="shared" si="0"/>
         <v>3.93</v>
       </c>
-      <c r="G18" s="156">
+      <c r="G18" s="128">
         <f>SUM(F18:F20)</f>
         <v>70.649999999999991</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="150">
+      <c r="A19" s="122">
         <v>3</v>
       </c>
-      <c r="B19" s="141">
-        <v>1</v>
-      </c>
-      <c r="C19" s="141" t="s">
+      <c r="B19" s="113">
+        <v>1</v>
+      </c>
+      <c r="C19" s="113" t="s">
         <v>0</v>
       </c>
-      <c r="D19" s="141">
+      <c r="D19" s="113">
         <v>5</v>
       </c>
-      <c r="E19" s="142">
+      <c r="E19" s="114">
         <v>5.56</v>
       </c>
-      <c r="F19" s="138">
-        <f>E19*D19</f>
+      <c r="F19" s="110">
+        <f t="shared" si="0"/>
         <v>27.799999999999997</v>
       </c>
-      <c r="G19" s="148">
+      <c r="G19" s="120">
         <f>SUM(F18:F20)</f>
         <v>70.649999999999991</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="194">
+      <c r="A20" s="166">
         <v>3</v>
       </c>
-      <c r="B20" s="195">
-        <v>1</v>
-      </c>
-      <c r="C20" s="195" t="s">
+      <c r="B20" s="167">
+        <v>1</v>
+      </c>
+      <c r="C20" s="167" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="195">
+      <c r="D20" s="167">
         <v>7</v>
       </c>
-      <c r="E20" s="196">
+      <c r="E20" s="168">
         <v>5.56</v>
       </c>
-      <c r="F20" s="160">
-        <f>E20*D20</f>
+      <c r="F20" s="132">
+        <f t="shared" si="0"/>
         <v>38.919999999999995</v>
       </c>
-      <c r="G20" s="161">
+      <c r="G20" s="133">
         <f>SUM(F18:F20)</f>
         <v>70.649999999999991</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="197">
+      <c r="A21" s="169">
         <v>3</v>
       </c>
-      <c r="B21" s="198">
-        <v>2</v>
-      </c>
-      <c r="C21" s="198" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="198">
+      <c r="B21" s="170">
+        <v>2</v>
+      </c>
+      <c r="C21" s="170" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="170">
         <v>10</v>
       </c>
-      <c r="E21" s="199">
+      <c r="E21" s="171">
         <v>7.23</v>
       </c>
-      <c r="F21" s="146">
-        <f>E21*D21</f>
+      <c r="F21" s="118">
+        <f t="shared" si="0"/>
         <v>72.300000000000011</v>
       </c>
-      <c r="G21" s="147">
+      <c r="G21" s="119">
         <f>SUM(F21)</f>
         <v>72.300000000000011</v>
       </c>
@@ -2956,19 +3029,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D190C58-97B3-4FCC-8D31-8F1AF72C877A}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="13.44140625" customWidth="1"/>
     <col min="6" max="6" width="14.109375" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -2987,8 +3062,17 @@
       <c r="F1" s="85" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="209" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="206" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="22">
         <v>2</v>
       </c>
@@ -3004,11 +3088,23 @@
       <c r="E2" s="23">
         <v>1.31</v>
       </c>
-      <c r="F2" s="116">
+      <c r="F2" s="189">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" s="200">
+        <f>SUM(D2:D8)</f>
+        <v>13</v>
+      </c>
+      <c r="H2" s="200">
+        <f>SUM(I2:I8)</f>
+        <v>17.03</v>
+      </c>
+      <c r="I2" s="211">
+        <f>D2*E2</f>
+        <v>2.62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="86">
         <v>2</v>
       </c>
@@ -3024,9 +3120,15 @@
       <c r="E3" s="13">
         <v>1.31</v>
       </c>
-      <c r="F3" s="117"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F3" s="190"/>
+      <c r="G3" s="201"/>
+      <c r="H3" s="201"/>
+      <c r="I3" s="207">
+        <f t="shared" ref="I3:I21" si="0">D3*E3</f>
+        <v>2.62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="25">
         <v>2</v>
       </c>
@@ -3042,9 +3144,15 @@
       <c r="E4" s="26">
         <v>1.31</v>
       </c>
-      <c r="F4" s="117"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F4" s="190"/>
+      <c r="G4" s="201"/>
+      <c r="H4" s="201"/>
+      <c r="I4" s="207">
+        <f t="shared" si="0"/>
+        <v>3.93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="87">
         <v>3</v>
       </c>
@@ -3060,9 +3168,15 @@
       <c r="E5" s="88">
         <v>1.31</v>
       </c>
-      <c r="F5" s="117"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F5" s="190"/>
+      <c r="G5" s="201"/>
+      <c r="H5" s="201"/>
+      <c r="I5" s="207">
+        <f t="shared" si="0"/>
+        <v>3.93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="87">
         <v>4</v>
       </c>
@@ -3078,9 +3192,15 @@
       <c r="E6" s="88">
         <v>1.31</v>
       </c>
-      <c r="F6" s="117"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F6" s="190"/>
+      <c r="G6" s="201"/>
+      <c r="H6" s="201"/>
+      <c r="I6" s="207">
+        <f t="shared" si="0"/>
+        <v>1.31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="87">
         <v>4</v>
       </c>
@@ -3096,9 +3216,15 @@
       <c r="E7" s="88">
         <v>1.31</v>
       </c>
-      <c r="F7" s="117"/>
-    </row>
-    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F7" s="190"/>
+      <c r="G7" s="201"/>
+      <c r="H7" s="201"/>
+      <c r="I7" s="207">
+        <f t="shared" si="0"/>
+        <v>1.31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="87">
         <v>5</v>
       </c>
@@ -3114,9 +3240,15 @@
       <c r="E8" s="88">
         <v>1.31</v>
       </c>
-      <c r="F8" s="118"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F8" s="191"/>
+      <c r="G8" s="202"/>
+      <c r="H8" s="202"/>
+      <c r="I8" s="210">
+        <f t="shared" si="0"/>
+        <v>1.31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>1</v>
       </c>
@@ -3132,11 +3264,23 @@
       <c r="E9" s="94">
         <v>5.56</v>
       </c>
-      <c r="F9" s="119">
+      <c r="F9" s="193">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9" s="200">
+        <f>SUM(D9:D15)</f>
+        <v>27</v>
+      </c>
+      <c r="H9" s="200">
+        <f>SUM(I9:I15)</f>
+        <v>150.12</v>
+      </c>
+      <c r="I9" s="211">
+        <f t="shared" si="0"/>
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>2</v>
       </c>
@@ -3152,9 +3296,15 @@
       <c r="E10" s="94">
         <v>5.56</v>
       </c>
-      <c r="F10" s="119"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F10" s="192"/>
+      <c r="G10" s="201"/>
+      <c r="H10" s="201"/>
+      <c r="I10" s="207">
+        <f t="shared" si="0"/>
+        <v>22.24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>2</v>
       </c>
@@ -3170,9 +3320,15 @@
       <c r="E11" s="94">
         <v>5.56</v>
       </c>
-      <c r="F11" s="119"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F11" s="192"/>
+      <c r="G11" s="201"/>
+      <c r="H11" s="201"/>
+      <c r="I11" s="207">
+        <f t="shared" si="0"/>
+        <v>33.36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="28">
         <v>3</v>
       </c>
@@ -3188,9 +3344,15 @@
       <c r="E12" s="95">
         <v>5.56</v>
       </c>
-      <c r="F12" s="119"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F12" s="192"/>
+      <c r="G12" s="201"/>
+      <c r="H12" s="201"/>
+      <c r="I12" s="207">
+        <f t="shared" si="0"/>
+        <v>27.799999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="31">
         <v>3</v>
       </c>
@@ -3206,9 +3368,15 @@
       <c r="E13" s="33">
         <v>5.56</v>
       </c>
-      <c r="F13" s="119"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F13" s="192"/>
+      <c r="G13" s="201"/>
+      <c r="H13" s="201"/>
+      <c r="I13" s="207">
+        <f t="shared" si="0"/>
+        <v>38.919999999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>4</v>
       </c>
@@ -3224,9 +3392,15 @@
       <c r="E14" s="94">
         <v>5.56</v>
       </c>
-      <c r="F14" s="119"/>
-    </row>
-    <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F14" s="192"/>
+      <c r="G14" s="201"/>
+      <c r="H14" s="201"/>
+      <c r="I14" s="207">
+        <f t="shared" si="0"/>
+        <v>11.12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>5</v>
       </c>
@@ -3242,9 +3416,15 @@
       <c r="E15" s="94">
         <v>5.56</v>
       </c>
-      <c r="F15" s="119"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F15" s="194"/>
+      <c r="G15" s="202"/>
+      <c r="H15" s="202"/>
+      <c r="I15" s="210">
+        <f t="shared" si="0"/>
+        <v>11.12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="90">
         <v>1</v>
       </c>
@@ -3260,11 +3440,23 @@
       <c r="E16" s="96">
         <v>7.23</v>
       </c>
-      <c r="F16" s="120">
+      <c r="F16" s="193">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G16" s="204">
+        <f>SUM(D16:D19)</f>
+        <v>17</v>
+      </c>
+      <c r="H16" s="204">
+        <f>SUM(I16:I19)</f>
+        <v>122.91000000000001</v>
+      </c>
+      <c r="I16" s="211">
+        <f t="shared" si="0"/>
+        <v>14.46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="90">
         <v>1</v>
       </c>
@@ -3280,9 +3472,15 @@
       <c r="E17" s="96">
         <v>7.23</v>
       </c>
-      <c r="F17" s="119"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F17" s="192"/>
+      <c r="G17" s="203"/>
+      <c r="H17" s="203"/>
+      <c r="I17" s="207">
+        <f t="shared" si="0"/>
+        <v>28.92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="90">
         <v>3</v>
       </c>
@@ -3298,9 +3496,15 @@
       <c r="E18" s="96">
         <v>7.23</v>
       </c>
-      <c r="F18" s="119"/>
-    </row>
-    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F18" s="192"/>
+      <c r="G18" s="203"/>
+      <c r="H18" s="203"/>
+      <c r="I18" s="207">
+        <f t="shared" si="0"/>
+        <v>72.300000000000011</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="90">
         <v>4</v>
       </c>
@@ -3316,9 +3520,15 @@
       <c r="E19" s="96">
         <v>7.23</v>
       </c>
-      <c r="F19" s="121"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F19" s="194"/>
+      <c r="G19" s="205"/>
+      <c r="H19" s="205"/>
+      <c r="I19" s="210">
+        <f t="shared" si="0"/>
+        <v>7.23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="92">
         <v>5</v>
       </c>
@@ -3334,11 +3544,23 @@
       <c r="E20" s="97">
         <v>4.2</v>
       </c>
-      <c r="F20" s="119">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F20" s="192">
+        <v>2</v>
+      </c>
+      <c r="G20" s="203">
+        <f>SUM(D20:D21)</f>
+        <v>7</v>
+      </c>
+      <c r="H20" s="203">
+        <f>SUM(I20:I21)</f>
+        <v>29.4</v>
+      </c>
+      <c r="I20" s="208">
+        <f t="shared" si="0"/>
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
         <v>6</v>
       </c>
@@ -3354,10 +3576,20 @@
       <c r="E21" s="42">
         <v>4.2</v>
       </c>
-      <c r="F21" s="121"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F21" s="194"/>
+      <c r="G21" s="205"/>
+      <c r="H21" s="205"/>
+      <c r="I21" s="210">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F22" s="98"/>
+      <c r="H22">
+        <f>SUM(H2:H21)</f>
+        <v>319.45999999999998</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A25:E44">
@@ -3366,11 +3598,19 @@
     <sortCondition ref="B25:B44"/>
     <sortCondition ref="D25:D44"/>
   </sortState>
-  <mergeCells count="4">
+  <mergeCells count="12">
+    <mergeCell ref="H2:H8"/>
+    <mergeCell ref="H9:H15"/>
+    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="H20:H21"/>
     <mergeCell ref="F2:F8"/>
     <mergeCell ref="F9:F15"/>
     <mergeCell ref="F16:F19"/>
     <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G2:G8"/>
+    <mergeCell ref="G9:G15"/>
+    <mergeCell ref="G16:G19"/>
+    <mergeCell ref="G20:G21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3447,7 +3687,7 @@
       <c r="E3" s="24">
         <v>7.23</v>
       </c>
-      <c r="F3" s="122">
+      <c r="F3" s="195">
         <v>2</v>
       </c>
     </row>
@@ -3467,7 +3707,7 @@
       <c r="E4" s="27">
         <v>7.23</v>
       </c>
-      <c r="F4" s="123"/>
+      <c r="F4" s="196"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="28">
@@ -3485,7 +3725,7 @@
       <c r="E5" s="29">
         <v>1.31</v>
       </c>
-      <c r="F5" s="122">
+      <c r="F5" s="195">
         <v>1</v>
       </c>
     </row>
@@ -3505,7 +3745,7 @@
       <c r="E6" s="14">
         <v>1.31</v>
       </c>
-      <c r="F6" s="124"/>
+      <c r="F6" s="197"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="31">
@@ -3523,7 +3763,7 @@
       <c r="E7" s="32">
         <v>1.31</v>
       </c>
-      <c r="F7" s="123"/>
+      <c r="F7" s="196"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="75">
@@ -3541,7 +3781,7 @@
       <c r="E8" s="15">
         <v>5.56</v>
       </c>
-      <c r="F8" s="125">
+      <c r="F8" s="198">
         <v>2</v>
       </c>
     </row>
@@ -3561,7 +3801,7 @@
       <c r="E9" s="15">
         <v>5.56</v>
       </c>
-      <c r="F9" s="126"/>
+      <c r="F9" s="199"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="90">
@@ -3599,7 +3839,7 @@
       <c r="E11" s="100">
         <v>5.56</v>
       </c>
-      <c r="F11" s="125">
+      <c r="F11" s="198">
         <v>1</v>
       </c>
     </row>
@@ -3619,7 +3859,7 @@
       <c r="E12" s="38">
         <v>5.56</v>
       </c>
-      <c r="F12" s="126"/>
+      <c r="F12" s="199"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="57">
@@ -3657,7 +3897,7 @@
       <c r="E14" s="40">
         <v>1.31</v>
       </c>
-      <c r="F14" s="125">
+      <c r="F14" s="198">
         <v>2</v>
       </c>
     </row>
@@ -3677,7 +3917,7 @@
       <c r="E15" s="41">
         <v>1.31</v>
       </c>
-      <c r="F15" s="126"/>
+      <c r="F15" s="199"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="92">

</xml_diff>